<commit_message>
added that will never work to finished book list
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E22AE61D-F22C-44D7-AF65-DE4263F7EB36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0C7BB6-6E05-4E8E-A14B-2AD28DE61AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25020" yWindow="2415" windowWidth="7500" windowHeight="6000" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>beanie babies;bubble;mania;biography;Ty Warner</t>
+  </si>
+  <si>
+    <t>That Will Never Work</t>
+  </si>
+  <si>
+    <t>Marc Randolph</t>
+  </si>
+  <si>
+    <t>netflix;startups;business;ipo;technology</t>
   </si>
 </sst>
 </file>
@@ -416,22 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -465,7 +474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -480,6 +489,23 @@
       </c>
       <c r="E3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43833</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43835</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Type, Length columns. addded An Elegant Defense
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0C7BB6-6E05-4E8E-A14B-2AD28DE61AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E37A5D-6DFA-440C-98A1-AD93D4418078}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -73,6 +73,39 @@
   </si>
   <si>
     <t>netflix;startups;business;ipo;technology</t>
+  </si>
+  <si>
+    <t>An Elegant Defense</t>
+  </si>
+  <si>
+    <t>Matt Richtel</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Hard Copy</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>immunology;health;medicine</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>8 Hrs 36 Mins</t>
+  </si>
+  <si>
+    <t>12 Hrs 38 Mins</t>
+  </si>
+  <si>
+    <t>337 Pages</t>
+  </si>
+  <si>
+    <t>304 Pages</t>
   </si>
 </sst>
 </file>
@@ -425,22 +458,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +491,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -473,8 +514,14 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -490,8 +537,14 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -506,6 +559,35 @@
       </c>
       <c r="E4" t="s">
         <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43832</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43840</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added make your bed
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6306A91-4865-4A12-9A9F-0CFAA4F2D114}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9027733E-DFEB-4D62-AE0D-170DC71C81E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>383 Pages</t>
+  </si>
+  <si>
+    <t>Make Your Bed</t>
+  </si>
+  <si>
+    <t>William H. McRaven</t>
+  </si>
+  <si>
+    <t>inspiration;success;self-improvement;motivation</t>
+  </si>
+  <si>
+    <t>125 Pages</t>
   </si>
 </sst>
 </file>
@@ -470,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,6 +637,29 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43841</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43842</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added living with a seal
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9027733E-DFEB-4D62-AE0D-170DC71C81E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1FAC6-EB39-4BF7-9D3C-5E3C8E5602FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>125 Pages</t>
+  </si>
+  <si>
+    <t>Living With a SEAL</t>
+  </si>
+  <si>
+    <t>Jesse Itzler</t>
+  </si>
+  <si>
+    <t>exercise;motivation;self-improvement</t>
+  </si>
+  <si>
+    <t>5 Hrs 19 Mins</t>
   </si>
 </sst>
 </file>
@@ -482,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,6 +672,29 @@
         <v>32</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43840</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43842</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a Books I want to read tab
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1FAC6-EB39-4BF7-9D3C-5E3C8E5602FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CD44D2-8605-4E60-B84A-E5F3621F3C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Completed" sheetId="1" r:id="rId1"/>
+    <sheet name="Books I want to read" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>Title</t>
   </si>
@@ -142,6 +143,126 @@
   </si>
   <si>
     <t>5 Hrs 19 Mins</t>
+  </si>
+  <si>
+    <t>Bird by Bird: Some Instructions on Writing and Life</t>
+  </si>
+  <si>
+    <t>Anne Lamott</t>
+  </si>
+  <si>
+    <t>David McCullough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columbine </t>
+  </si>
+  <si>
+    <t>Dave Cullen</t>
+  </si>
+  <si>
+    <t>Hidden Figures</t>
+  </si>
+  <si>
+    <t>Margot Lee Shetterly</t>
+  </si>
+  <si>
+    <t>A People's History of the United States</t>
+  </si>
+  <si>
+    <t>Howard Zinn</t>
+  </si>
+  <si>
+    <t>S.P.Q.R A History of Ancient Rome</t>
+  </si>
+  <si>
+    <t>Mary Beard</t>
+  </si>
+  <si>
+    <t>The Immortal Life of Henrietta Lacks</t>
+  </si>
+  <si>
+    <t>Rebecca Skloot</t>
+  </si>
+  <si>
+    <t>True North: Discover your authentic leadership</t>
+  </si>
+  <si>
+    <t>Bill George</t>
+  </si>
+  <si>
+    <t>The Money of Invention: How Venture Capital Creates New Wealth</t>
+  </si>
+  <si>
+    <t>Paul Gompers + Josh Lerner</t>
+  </si>
+  <si>
+    <t>Many Unhappy Returns: One Man's Quest to Turn Around the Most Unpopular Organization in America</t>
+  </si>
+  <si>
+    <t>Charles O. Rossotti</t>
+  </si>
+  <si>
+    <t>Unleashing Innovation: How Whirlpool Transformed an Industry</t>
+  </si>
+  <si>
+    <t>Nancy Tennant Snyder</t>
+  </si>
+  <si>
+    <t>Scaling Up Excellence: Getting to More Without Settling for Less</t>
+  </si>
+  <si>
+    <t>Robert Sutton + Huggy Rao</t>
+  </si>
+  <si>
+    <t>Idea Man</t>
+  </si>
+  <si>
+    <t>Paul Allen</t>
+  </si>
+  <si>
+    <t>My Fathers Business: The small-town values that built dollar general into a billion-dollar company</t>
+  </si>
+  <si>
+    <t>Cal Turner Jr</t>
+  </si>
+  <si>
+    <t>The Undertaking: Life Studies from the Dismal Trade</t>
+  </si>
+  <si>
+    <t>Thomas Lynch</t>
+  </si>
+  <si>
+    <t>Growing A Business</t>
+  </si>
+  <si>
+    <t>Paul Hawken</t>
+  </si>
+  <si>
+    <t>Personal History</t>
+  </si>
+  <si>
+    <t>Katharine Graham</t>
+  </si>
+  <si>
+    <t>Tough Choices</t>
+  </si>
+  <si>
+    <t>Carly Fiorina</t>
+  </si>
+  <si>
+    <t>Rising to the Challenge: My Leadership Journey</t>
+  </si>
+  <si>
+    <t>Setting the Table</t>
+  </si>
+  <si>
+    <t>Danny Meyer</t>
+  </si>
+  <si>
+    <t>Iacocca</t>
+  </si>
+  <si>
+    <t>Lee Iacocca</t>
   </si>
 </sst>
 </file>
@@ -177,9 +298,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -698,4 +822,199 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDDD9D0-399A-4972-B572-FF4C9ED18E5D}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1776</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added the first 20 minutes and start of mindset
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFC9D97-64A5-47FF-801D-F017FCED773B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80C59A7-445D-41AC-932C-CBE231D2ACD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Title</t>
   </si>
@@ -275,6 +275,30 @@
   </si>
   <si>
     <t>6 Hrs 32 Mins</t>
+  </si>
+  <si>
+    <t>The First 20 Minutes</t>
+  </si>
+  <si>
+    <t>Gretchen Reynolds</t>
+  </si>
+  <si>
+    <t>exercise;science;biology;health;fitness</t>
+  </si>
+  <si>
+    <t>9 Hrs 7 Mins</t>
+  </si>
+  <si>
+    <t>Mindset</t>
+  </si>
+  <si>
+    <t>Carol Dweck</t>
+  </si>
+  <si>
+    <t>psychology;self-improvement;growth mindset;fixed mindset</t>
+  </si>
+  <si>
+    <t>320 Pages</t>
   </si>
 </sst>
 </file>
@@ -630,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -852,6 +876,49 @@
       </c>
       <c r="G9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43843</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43846</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43842</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added end date for mindset and how we learn
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80C59A7-445D-41AC-932C-CBE231D2ACD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C189FB45-D9A2-40D2-A8E1-4912947FB2B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
   <si>
     <t>Title</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>320 Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How We Learn </t>
+  </si>
+  <si>
+    <t>Benedict Carey</t>
+  </si>
+  <si>
+    <t>learning;psychology;science;neurology</t>
+  </si>
+  <si>
+    <t>7 Hrs 21 Mins</t>
   </si>
 </sst>
 </file>
@@ -654,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,6 +923,9 @@
       <c r="C11" s="1">
         <v>43842</v>
       </c>
+      <c r="D11" s="1">
+        <v>43847</v>
+      </c>
       <c r="E11" t="s">
         <v>87</v>
       </c>
@@ -919,6 +934,29 @@
       </c>
       <c r="G11" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43846</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43847</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pioneers and beginnings of Iaccoca
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C189FB45-D9A2-40D2-A8E1-4912947FB2B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE94DC3-DD49-4D65-9249-F6D89FF107CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>Title</t>
   </si>
@@ -311,6 +311,24 @@
   </si>
   <si>
     <t>7 Hrs 21 Mins</t>
+  </si>
+  <si>
+    <t>The Pioneers</t>
+  </si>
+  <si>
+    <t>history;ohio;pioneers;america;1700s;1800s</t>
+  </si>
+  <si>
+    <t>10 Hrs 33 Mins</t>
+  </si>
+  <si>
+    <t>Iaccoca: An Autobiography</t>
+  </si>
+  <si>
+    <t>Lee Iaccoca</t>
+  </si>
+  <si>
+    <t>memoir;business;ford;chrysler;Lee Iaccoca</t>
   </si>
 </sst>
 </file>
@@ -666,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,6 +975,46 @@
       </c>
       <c r="G12" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43847</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43850</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43847</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sports gene and leadership gap
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE94DC3-DD49-4D65-9249-F6D89FF107CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD295E86-9386-4C95-8C2A-1063CD786A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="107">
   <si>
     <t>Title</t>
   </si>
@@ -329,6 +329,30 @@
   </si>
   <si>
     <t>memoir;business;ford;chrysler;Lee Iaccoca</t>
+  </si>
+  <si>
+    <t>The Sports Gene</t>
+  </si>
+  <si>
+    <t>David Epstein</t>
+  </si>
+  <si>
+    <t>sports;science;genetics;expertise</t>
+  </si>
+  <si>
+    <t>The Leadership Gap</t>
+  </si>
+  <si>
+    <t>Lolly Daskal</t>
+  </si>
+  <si>
+    <t>leadership;success;self-improvement</t>
+  </si>
+  <si>
+    <t>6 Hrs 18 Mins</t>
+  </si>
+  <si>
+    <t>10 Hrs 23 Mins</t>
   </si>
 </sst>
 </file>
@@ -684,24 +708,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -747,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -770,7 +794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -793,7 +817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -816,7 +840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -839,7 +863,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -862,7 +886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -885,7 +909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -908,7 +932,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -931,7 +955,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -954,7 +978,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -977,7 +1001,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1000,7 +1024,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -1015,6 +1039,52 @@
       </c>
       <c r="F14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43850</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43853</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43853</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43854</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1030,13 +1100,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1052,7 +1122,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -1060,7 +1130,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1068,7 +1138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1076,7 +1146,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1084,7 +1154,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -1092,7 +1162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1100,7 +1170,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1108,7 +1178,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1116,7 +1186,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1124,7 +1194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1132,7 +1202,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1140,7 +1210,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1148,7 +1218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1156,7 +1226,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1164,7 +1234,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1172,7 +1242,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1180,7 +1250,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1188,7 +1258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1196,7 +1266,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -1204,7 +1274,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added a marvelous life
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FC3210-AE45-480A-BDA3-65B505D755D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26E88B6-B485-4E76-92A5-F84E5C6484B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
   <si>
     <t>Title</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>341 Pages</t>
+  </si>
+  <si>
+    <t>A Marvelous Life</t>
+  </si>
+  <si>
+    <t>Danny Fingeroth</t>
+  </si>
+  <si>
+    <t>biography;marvel;stan lee;comics</t>
+  </si>
+  <si>
+    <t>14 Hrs 47 Mins</t>
   </si>
 </sst>
 </file>
@@ -711,7 +723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
@@ -1094,6 +1106,29 @@
       </c>
       <c r="G16" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43853</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43859</v>
+      </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added jim koch book and how chefs holiday
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26E88B6-B485-4E76-92A5-F84E5C6484B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E20E64A-3DEE-400C-BA14-92D16ED087F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
   <si>
     <t>Title</t>
   </si>
@@ -368,6 +368,30 @@
   </si>
   <si>
     <t>14 Hrs 47 Mins</t>
+  </si>
+  <si>
+    <t>Quench Your Own Thirst</t>
+  </si>
+  <si>
+    <t>Jim Koch</t>
+  </si>
+  <si>
+    <t>biography;business;sam adams;brewing;beer</t>
+  </si>
+  <si>
+    <t>7 Hrs 31 Mins</t>
+  </si>
+  <si>
+    <t>How Chefs Holiday</t>
+  </si>
+  <si>
+    <t>Dana Cowin</t>
+  </si>
+  <si>
+    <t>chefs;food;cooking;holidays</t>
+  </si>
+  <si>
+    <t>1 Hour 1 Min</t>
   </si>
 </sst>
 </file>
@@ -723,24 +747,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -786,7 +810,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -809,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -832,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -855,7 +879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -878,7 +902,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -901,7 +925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -924,7 +948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -947,7 +971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -970,7 +994,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -993,7 +1017,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1016,7 +1040,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1039,7 +1063,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -1062,7 +1086,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1085,7 +1109,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -1108,7 +1132,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1129,6 +1153,52 @@
       </c>
       <c r="G17" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43859</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43861</v>
+      </c>
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43861</v>
+      </c>
+      <c r="D19" s="1">
+        <v>43861</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1144,13 +1214,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1166,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -1174,7 +1244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1182,7 +1252,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1190,7 +1260,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1198,7 +1268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -1206,7 +1276,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1214,7 +1284,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1222,7 +1292,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1230,7 +1300,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1238,7 +1308,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1246,7 +1316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1254,7 +1324,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1262,7 +1332,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1270,7 +1340,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1278,7 +1348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1286,7 +1356,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1294,7 +1364,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1302,7 +1372,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1310,7 +1380,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -1318,7 +1388,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added a place holder for deep learning
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C1CD3-CB92-47CD-A278-F4C349318B07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E7423-2AEB-494A-A326-EF5903066CC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="142">
   <si>
     <t>Title</t>
   </si>
@@ -449,6 +449,15 @@
   </si>
   <si>
     <t>25 Hours 15 Mins</t>
+  </si>
+  <si>
+    <t>Deep Learning</t>
+  </si>
+  <si>
+    <t>deep learning;machine learning;data science;neural networks</t>
+  </si>
+  <si>
+    <t>Ebook</t>
   </si>
 </sst>
 </file>
@@ -804,24 +813,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -867,7 +876,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -890,7 +899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -913,7 +922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -936,7 +945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -959,7 +968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -982,7 +991,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1051,7 +1060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -1143,7 +1152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -1189,7 +1198,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -1304,7 +1313,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -1350,7 +1359,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -1371,6 +1380,20 @@
       </c>
       <c r="G24" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43874</v>
+      </c>
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1386,13 +1409,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1400,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1408,7 +1431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -1416,7 +1439,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1424,7 +1447,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1432,7 +1455,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1463,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -1448,7 +1471,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1456,7 +1479,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1464,7 +1487,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1472,7 +1495,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1480,7 +1503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +1511,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1519,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1504,7 +1527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1512,7 +1535,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1520,7 +1543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1528,7 +1551,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1536,7 +1559,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1544,7 +1567,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1552,7 +1575,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -1560,7 +1583,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added why we sleep
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E7423-2AEB-494A-A326-EF5903066CC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45128554-E7A5-4C52-9A24-345FAC7ACBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="146">
   <si>
     <t>Title</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>Ebook</t>
+  </si>
+  <si>
+    <t>Why We Sleep</t>
+  </si>
+  <si>
+    <t>Matthew Walker</t>
+  </si>
+  <si>
+    <t>sleep;health;science;sleep deprivation;disease;wellness</t>
+  </si>
+  <si>
+    <t>14 Hours 0 Mins</t>
   </si>
 </sst>
 </file>
@@ -813,24 +825,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -876,7 +888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -899,7 +911,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -922,7 +934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -945,7 +957,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -968,7 +980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1037,7 +1049,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1106,7 +1118,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1129,7 +1141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1175,7 +1187,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -1198,7 +1210,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1221,7 +1233,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1267,7 +1279,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -1382,7 +1394,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -1394,6 +1406,29 @@
       </c>
       <c r="F25" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43876</v>
+      </c>
+      <c r="D26" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1409,13 +1444,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1431,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -1439,7 +1474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1447,7 +1482,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1455,7 +1490,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1498,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -1471,7 +1506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1479,7 +1514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1487,7 +1522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1495,7 +1530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1538,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1511,7 +1546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1519,7 +1554,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1527,7 +1562,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1535,7 +1570,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1543,7 +1578,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1551,7 +1586,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1559,7 +1594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1567,7 +1602,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1575,7 +1610,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -1583,7 +1618,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added trillion dollar coach
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45128554-E7A5-4C52-9A24-345FAC7ACBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5ED486-B8CC-47B5-8BA1-110507911A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="150">
   <si>
     <t>Title</t>
   </si>
@@ -470,6 +470,18 @@
   </si>
   <si>
     <t>14 Hours 0 Mins</t>
+  </si>
+  <si>
+    <t>Trillion Dollar Coach</t>
+  </si>
+  <si>
+    <t>Alan Eagle;Eric Schmidt;Jonathan Rosenberg</t>
+  </si>
+  <si>
+    <t>coaching;management;team building;bill campbell;google;silicon valley</t>
+  </si>
+  <si>
+    <t>5 Hours 40 Mins</t>
   </si>
 </sst>
 </file>
@@ -825,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1429,6 +1441,29 @@
       </c>
       <c r="G26" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43879</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43879</v>
+      </c>
+      <c r="E27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cant hurt me data
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5ED486-B8CC-47B5-8BA1-110507911A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABFCF9B-ADD9-4E77-9D4C-82447442161B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
   <si>
     <t>Title</t>
   </si>
@@ -482,6 +482,15 @@
   </si>
   <si>
     <t>5 Hours 40 Mins</t>
+  </si>
+  <si>
+    <t>Can't Hurt Me</t>
+  </si>
+  <si>
+    <t>David Goggins</t>
+  </si>
+  <si>
+    <t>david goggins;no weakness;mental toughness;fitness;strong;navy seals</t>
   </si>
 </sst>
 </file>
@@ -837,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1464,6 +1473,23 @@
       </c>
       <c r="G27" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43879</v>
+      </c>
+      <c r="E28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added spqr and finished cant hurt me
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABFCF9B-ADD9-4E77-9D4C-82447442161B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4EFF28-B6B9-4D52-8F77-920690110058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="157">
   <si>
     <t>Title</t>
   </si>
@@ -491,6 +491,18 @@
   </si>
   <si>
     <t>david goggins;no weakness;mental toughness;fitness;strong;navy seals</t>
+  </si>
+  <si>
+    <t>13 Hours 37 Mins</t>
+  </si>
+  <si>
+    <t>SPQR</t>
+  </si>
+  <si>
+    <t>rome;history;romulus;remus;julius caesar;augustus;republic;empire;ancient history</t>
+  </si>
+  <si>
+    <t>536 Pages</t>
   </si>
 </sst>
 </file>
@@ -846,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1485,11 +1497,40 @@
       <c r="C28" s="1">
         <v>43879</v>
       </c>
+      <c r="D28" s="1">
+        <v>43880</v>
+      </c>
       <c r="E28" t="s">
         <v>152</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43867</v>
+      </c>
+      <c r="D29" s="1">
+        <v>43880</v>
+      </c>
+      <c r="E29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added house of morgan
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4EFF28-B6B9-4D52-8F77-920690110058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6FBE6C-CA27-4D04-A7E7-DE29180F5AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="161">
   <si>
     <t>Title</t>
   </si>
@@ -503,6 +503,18 @@
   </si>
   <si>
     <t>536 Pages</t>
+  </si>
+  <si>
+    <t>The House of Morgan</t>
+  </si>
+  <si>
+    <t>Ron Chernow</t>
+  </si>
+  <si>
+    <t>finance;history;jp morgan;jack morgan;great depression;investment banking;history</t>
+  </si>
+  <si>
+    <t>34 Hours 37 Mins</t>
   </si>
 </sst>
 </file>
@@ -858,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1531,6 +1543,29 @@
       </c>
       <c r="G29" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="1">
+        <v>43881</v>
+      </c>
+      <c r="D30" s="1">
+        <v>43888</v>
+      </c>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added crazy rich and deep work
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B949CF-539F-4EA6-9B95-AAC686CB7714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BEC21C-A111-4D94-ADEB-195943B70599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="173">
   <si>
     <t>Title</t>
   </si>
@@ -527,6 +527,30 @@
   </si>
   <si>
     <t>6 Hours 13 Mins</t>
+  </si>
+  <si>
+    <t>Deep Work</t>
+  </si>
+  <si>
+    <t>Cal Newport</t>
+  </si>
+  <si>
+    <t>self improvement;productivity;excellence;focus</t>
+  </si>
+  <si>
+    <t>Crazy Rich</t>
+  </si>
+  <si>
+    <t>Jerry Oppenheimer</t>
+  </si>
+  <si>
+    <t>dynasty;johnson &amp; johnson;heirs;scandal;history</t>
+  </si>
+  <si>
+    <t>15 Hours 13 Mins</t>
+  </si>
+  <si>
+    <t>7 Hours 44 Mins</t>
   </si>
 </sst>
 </file>
@@ -882,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,6 +1625,52 @@
       </c>
       <c r="G31" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43888</v>
+      </c>
+      <c r="D32" s="1">
+        <v>43889</v>
+      </c>
+      <c r="E32" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="1">
+        <v>43889</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43892</v>
+      </c>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added infinite powers, 4 hour work week and elizabeth II
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E053A5A-BCF4-43B2-9485-38375C1BFBDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35ED2D4-BA51-43F3-AC24-7EF1AB15E8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="189">
   <si>
     <t>Title</t>
   </si>
@@ -563,6 +563,42 @@
   </si>
   <si>
     <t>sugar;slavery;obesity;america;industry;health;history</t>
+  </si>
+  <si>
+    <t>Infinite Powers</t>
+  </si>
+  <si>
+    <t>Steven Strogatz</t>
+  </si>
+  <si>
+    <t>math;calculus;infinity;history;newton</t>
+  </si>
+  <si>
+    <t>301 Pages</t>
+  </si>
+  <si>
+    <t>The 4-Hour Work Week</t>
+  </si>
+  <si>
+    <t>Tim Ferris</t>
+  </si>
+  <si>
+    <t>fullfillment;self improvement;productivity</t>
+  </si>
+  <si>
+    <t>13 Hours 1 Min</t>
+  </si>
+  <si>
+    <t>Elizabeth II: Life of a Monarch</t>
+  </si>
+  <si>
+    <t>Ruth Cowen</t>
+  </si>
+  <si>
+    <t>queen Elizabeth;monarchy;biography;england;history</t>
+  </si>
+  <si>
+    <t>3 Hours 47 Mins</t>
   </si>
 </sst>
 </file>
@@ -918,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1706,6 +1742,75 @@
       </c>
       <c r="G34" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="1">
+        <v>43881</v>
+      </c>
+      <c r="D35" s="1">
+        <v>43897</v>
+      </c>
+      <c r="E35" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="1">
+        <v>43895</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43897</v>
+      </c>
+      <c r="E36" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="1">
+        <v>43901</v>
+      </c>
+      <c r="D37" s="1">
+        <v>43902</v>
+      </c>
+      <c r="E37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the leadership challenge
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35ED2D4-BA51-43F3-AC24-7EF1AB15E8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB8F634-C00F-4B1E-AA23-E73655993B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
   <si>
     <t>Title</t>
   </si>
@@ -599,6 +599,15 @@
   </si>
   <si>
     <t>3 Hours 47 Mins</t>
+  </si>
+  <si>
+    <t>The Leadership Challenge</t>
+  </si>
+  <si>
+    <t>Barry Posner;James Kouzes</t>
+  </si>
+  <si>
+    <t>11 Hours 1 Min</t>
   </si>
 </sst>
 </file>
@@ -954,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1811,6 +1820,29 @@
       </c>
       <c r="G37" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="1">
+        <v>43904</v>
+      </c>
+      <c r="D38" s="1">
+        <v>43906</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generation friends and american icon
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB8F634-C00F-4B1E-AA23-E73655993B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62ACE54-5C2E-431C-9DF8-FE40BC8DC514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="199">
   <si>
     <t>Title</t>
   </si>
@@ -608,6 +608,27 @@
   </si>
   <si>
     <t>11 Hours 1 Min</t>
+  </si>
+  <si>
+    <t>Generation Friends</t>
+  </si>
+  <si>
+    <t>Saul Austerlitz</t>
+  </si>
+  <si>
+    <t>friends;tv;hollywood;history;analysis</t>
+  </si>
+  <si>
+    <t>American Icon</t>
+  </si>
+  <si>
+    <t>Bryce G. Hoffman</t>
+  </si>
+  <si>
+    <t>alan mulally;ford;great recession;business;turn around; history;success</t>
+  </si>
+  <si>
+    <t>398 Pages</t>
   </si>
 </sst>
 </file>
@@ -963,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1843,6 +1864,52 @@
       </c>
       <c r="G38" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="1">
+        <v>43907</v>
+      </c>
+      <c r="D39" s="1">
+        <v>43910</v>
+      </c>
+      <c r="E39" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="1">
+        <v>43898</v>
+      </c>
+      <c r="D40" s="1">
+        <v>43911</v>
+      </c>
+      <c r="E40" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in defense of elitism
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62ACE54-5C2E-431C-9DF8-FE40BC8DC514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116ECF0-C970-4A99-A9AD-C11D7CBC02D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="203">
   <si>
     <t>Title</t>
   </si>
@@ -629,6 +629,18 @@
   </si>
   <si>
     <t>398 Pages</t>
+  </si>
+  <si>
+    <t>7 Hours 19 Mins</t>
+  </si>
+  <si>
+    <t>In Defense of Elitism</t>
+  </si>
+  <si>
+    <t>Joel Stein</t>
+  </si>
+  <si>
+    <t>elitism;academics;populism;politics</t>
   </si>
 </sst>
 </file>
@@ -984,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1910,6 +1922,29 @@
       </c>
       <c r="G40" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="1">
+        <v>43910</v>
+      </c>
+      <c r="D41" s="1">
+        <v>43912</v>
+      </c>
+      <c r="E41" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added this is going to hurt
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116ECF0-C970-4A99-A9AD-C11D7CBC02D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDD6FA-4BA2-4D63-B838-49FB69760A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="207">
   <si>
     <t>Title</t>
   </si>
@@ -641,6 +641,18 @@
   </si>
   <si>
     <t>elitism;academics;populism;politics</t>
+  </si>
+  <si>
+    <t>This is Going to Hurt</t>
+  </si>
+  <si>
+    <t>Adam Kay</t>
+  </si>
+  <si>
+    <t>medicine;doctor;nhs;burnout;science</t>
+  </si>
+  <si>
+    <t>5 Hours 53 Mins</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1945,6 +1957,29 @@
       </c>
       <c r="G41" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" s="1">
+        <v>43912</v>
+      </c>
+      <c r="D42" s="1">
+        <v>43912</v>
+      </c>
+      <c r="E42" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added i am c3po and deep learning
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDD6FA-4BA2-4D63-B838-49FB69760A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5296790C-F54B-4C22-86BD-3FCA4C44FC2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="213">
   <si>
     <t>Title</t>
   </si>
@@ -653,6 +653,24 @@
   </si>
   <si>
     <t>5 Hours 53 Mins</t>
+  </si>
+  <si>
+    <t>I am C-3PO</t>
+  </si>
+  <si>
+    <t>Anthony Daniels</t>
+  </si>
+  <si>
+    <t>star wars;hollywood;movies;acting;c-3po</t>
+  </si>
+  <si>
+    <t>9 Hours 34 Mins</t>
+  </si>
+  <si>
+    <t>John D. Kellerher</t>
+  </si>
+  <si>
+    <t>250 Pages</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1980,6 +1998,52 @@
       </c>
       <c r="G42" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" s="1">
+        <v>43912</v>
+      </c>
+      <c r="D43" s="1">
+        <v>43913</v>
+      </c>
+      <c r="E43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>211</v>
+      </c>
+      <c r="C44" s="1">
+        <v>43911</v>
+      </c>
+      <c r="D44" s="1">
+        <v>43913</v>
+      </c>
+      <c r="E44" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added beyond these walls
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5296790C-F54B-4C22-86BD-3FCA4C44FC2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50147DE9-C0DB-430C-9016-78E7CEF3D40E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
   <si>
     <t>Title</t>
   </si>
@@ -671,6 +671,18 @@
   </si>
   <si>
     <t>250 Pages</t>
+  </si>
+  <si>
+    <t>Beyond These Walls</t>
+  </si>
+  <si>
+    <t>Tony Platt</t>
+  </si>
+  <si>
+    <t>crime;prison reform;criminal justice;policing</t>
+  </si>
+  <si>
+    <t>255 Pages</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2044,6 +2056,29 @@
       </c>
       <c r="G44" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D45" s="1">
+        <v>43918</v>
+      </c>
+      <c r="E45" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added kitchen confidential and get your shit together
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABBB2BE-CD2C-4132-9192-5438D482CFE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B44B59-E5FF-41B6-AA0D-5ED03D68CB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="229">
   <si>
     <t>Title</t>
   </si>
@@ -694,7 +694,31 @@
     <t>biography;arnold;success;body building;acting;business;politics</t>
   </si>
   <si>
-    <t>23 Hours 21 Min</t>
+    <t>Kitchen Confidential</t>
+  </si>
+  <si>
+    <t>Anthony Bourdain</t>
+  </si>
+  <si>
+    <t>cooking;chef;restaurants;</t>
+  </si>
+  <si>
+    <t>Get Your Shit Together</t>
+  </si>
+  <si>
+    <t>Sarah Knight</t>
+  </si>
+  <si>
+    <t>self help;productivity;focus;improvement</t>
+  </si>
+  <si>
+    <t>4 Hours 35 Mins</t>
+  </si>
+  <si>
+    <t>8 Hours 26 Mins</t>
+  </si>
+  <si>
+    <t>23 Hours 21 Mins</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2113,7 +2137,53 @@
         <v>16</v>
       </c>
       <c r="G46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>220</v>
+      </c>
+      <c r="B47" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="1">
+        <v>43919</v>
+      </c>
+      <c r="D47" s="1">
+        <v>43920</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" s="1">
+        <v>43920</v>
+      </c>
+      <c r="D48" s="1">
+        <v>43920</v>
+      </c>
+      <c r="E48" t="s">
+        <v>225</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the rise and fall of dinosaurs
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B44B59-E5FF-41B6-AA0D-5ED03D68CB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373ECBC2-B548-4880-B61D-82D5B37F2519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="233">
   <si>
     <t>Title</t>
   </si>
@@ -719,6 +719,18 @@
   </si>
   <si>
     <t>23 Hours 21 Mins</t>
+  </si>
+  <si>
+    <t>The Rise and Fall of the Dinosaurs</t>
+  </si>
+  <si>
+    <t>Steve Brusatte;Patrick Lawlor</t>
+  </si>
+  <si>
+    <t>dinosaurs;science;history</t>
+  </si>
+  <si>
+    <t>10 Hours 12 Mins</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,6 +2196,29 @@
       </c>
       <c r="G48" t="s">
         <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" s="1">
+        <v>43921</v>
+      </c>
+      <c r="D49" s="1">
+        <v>43922</v>
+      </c>
+      <c r="E49" t="s">
+        <v>231</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added game changer and project paperclip
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FE98D4-2444-44CA-83AE-4D946136066B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60206E-D182-449D-A2D9-5E57717C3861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="244">
   <si>
     <t>Title</t>
   </si>
@@ -740,6 +740,30 @@
   </si>
   <si>
     <t>8 Hours 59 Mins</t>
+  </si>
+  <si>
+    <t>Game-Changer</t>
+  </si>
+  <si>
+    <t>David McAdams</t>
+  </si>
+  <si>
+    <t>Game theory;economics;strategy</t>
+  </si>
+  <si>
+    <t>238 Pages</t>
+  </si>
+  <si>
+    <t>Operation Paperclip</t>
+  </si>
+  <si>
+    <t>Annie Jacobsen</t>
+  </si>
+  <si>
+    <t>nazis;history;science;holocaust;classified operations</t>
+  </si>
+  <si>
+    <t>19 Hours 26 Mins</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2251,6 +2275,52 @@
       </c>
       <c r="G50" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51" s="1">
+        <v>43927</v>
+      </c>
+      <c r="D51" s="1">
+        <v>43930</v>
+      </c>
+      <c r="E51" t="s">
+        <v>238</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="1">
+        <v>43927</v>
+      </c>
+      <c r="D52" s="1">
+        <v>43930</v>
+      </c>
+      <c r="E52" t="s">
+        <v>242</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added facebook the inside story
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60206E-D182-449D-A2D9-5E57717C3861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA960352-2A49-4CFE-B512-A22AC5592099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="248">
   <si>
     <t>Title</t>
   </si>
@@ -764,6 +764,18 @@
   </si>
   <si>
     <t>19 Hours 26 Mins</t>
+  </si>
+  <si>
+    <t>Facebook: The Inside Story</t>
+  </si>
+  <si>
+    <t>Steven Levy</t>
+  </si>
+  <si>
+    <t>facebook;entrepreuner;business;social networking;privacy;scandal</t>
+  </si>
+  <si>
+    <t>19 Hours 5 Mins</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2321,6 +2333,29 @@
       </c>
       <c r="G52" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>244</v>
+      </c>
+      <c r="B53" t="s">
+        <v>245</v>
+      </c>
+      <c r="C53" s="1">
+        <v>43930</v>
+      </c>
+      <c r="D53" s="1">
+        <v>43934</v>
+      </c>
+      <c r="E53" t="s">
+        <v>246</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added what it takes
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA960352-2A49-4CFE-B512-A22AC5592099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE5DBF-7FB5-4FC0-A51D-87DF6663A28A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="252">
   <si>
     <t>Title</t>
   </si>
@@ -776,6 +776,18 @@
   </si>
   <si>
     <t>19 Hours 5 Mins</t>
+  </si>
+  <si>
+    <t>What It Takes</t>
+  </si>
+  <si>
+    <t>Stephen Schwarzman</t>
+  </si>
+  <si>
+    <t>entreuprenuer;business;private equity;memoir;blackstone;investing;excellence</t>
+  </si>
+  <si>
+    <t>354 Pages</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2356,6 +2368,29 @@
       </c>
       <c r="G53" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" s="1">
+        <v>43931</v>
+      </c>
+      <c r="D54" s="1">
+        <v>43936</v>
+      </c>
+      <c r="E54" t="s">
+        <v>250</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the great influenza
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230D4116-AEF0-4620-95F6-049772F2E672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBF5CC0-457A-4F23-810D-8D6283B43944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="260">
   <si>
     <t>Title</t>
   </si>
@@ -800,6 +800,18 @@
   </si>
   <si>
     <t>164 Pages</t>
+  </si>
+  <si>
+    <t>The Great Influenza</t>
+  </si>
+  <si>
+    <t>John Barry;Scott Brick</t>
+  </si>
+  <si>
+    <t>influenza;pandemic;science;disease;history;spanish flu</t>
+  </si>
+  <si>
+    <t>19 Hours 34 Mins</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2426,6 +2438,29 @@
       </c>
       <c r="G55" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" t="s">
+        <v>257</v>
+      </c>
+      <c r="C56" s="1">
+        <v>43935</v>
+      </c>
+      <c r="D56" s="1">
+        <v>43939</v>
+      </c>
+      <c r="E56" t="s">
+        <v>258</v>
+      </c>
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delivering happiness and you do you
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBF5CC0-457A-4F23-810D-8D6283B43944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D547E93C-ABFE-4F87-88C8-F6517A08404E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="267">
   <si>
     <t>Title</t>
   </si>
@@ -812,6 +812,27 @@
   </si>
   <si>
     <t>19 Hours 34 Mins</t>
+  </si>
+  <si>
+    <t>Delivering Happiness</t>
+  </si>
+  <si>
+    <t>Tony Hsieh</t>
+  </si>
+  <si>
+    <t>zappos;entreuprenuer;business;start up</t>
+  </si>
+  <si>
+    <t>You Do You</t>
+  </si>
+  <si>
+    <t>self-improvement;happiness</t>
+  </si>
+  <si>
+    <t>8 Hours 22 Mins</t>
+  </si>
+  <si>
+    <t>5 Hours</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2461,6 +2482,52 @@
       </c>
       <c r="G56" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>260</v>
+      </c>
+      <c r="B57" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="1">
+        <v>43939</v>
+      </c>
+      <c r="D57" s="1">
+        <v>43940</v>
+      </c>
+      <c r="E57" t="s">
+        <v>262</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>263</v>
+      </c>
+      <c r="B58" t="s">
+        <v>224</v>
+      </c>
+      <c r="C58" s="1">
+        <v>43940</v>
+      </c>
+      <c r="D58" s="1">
+        <v>43940</v>
+      </c>
+      <c r="E58" t="s">
+        <v>264</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the little book of common sense investing
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B72186-E3D5-4D98-B70E-C185E3948A36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F873828-7A09-4EA5-A946-1297E6EFA041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="275">
   <si>
     <t>Title</t>
   </si>
@@ -845,6 +845,18 @@
   </si>
   <si>
     <t>10 Hours 29 Mins</t>
+  </si>
+  <si>
+    <t>The Little Book of Common Sense Investing</t>
+  </si>
+  <si>
+    <t>John C. Bogle</t>
+  </si>
+  <si>
+    <t>investing;stock market;index fund;passive investing</t>
+  </si>
+  <si>
+    <t>5 Hours 7 Mins</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2563,6 +2575,29 @@
       </c>
       <c r="G59" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" t="s">
+        <v>272</v>
+      </c>
+      <c r="C60" s="1">
+        <v>43942</v>
+      </c>
+      <c r="D60" s="1">
+        <v>43942</v>
+      </c>
+      <c r="E60" t="s">
+        <v>273</v>
+      </c>
+      <c r="F60" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added junkyard planet and the organized mind
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F295FECD-406D-4BE6-8339-CA6172CA0C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905B6BE9-9347-4269-A2FC-AD29CF0B773E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="286">
   <si>
     <t>Title</t>
   </si>
@@ -869,6 +869,27 @@
   </si>
   <si>
     <t>baseball;sabremetrics;data;analytics</t>
+  </si>
+  <si>
+    <t>Junkyard Planet</t>
+  </si>
+  <si>
+    <t>Adam Minter</t>
+  </si>
+  <si>
+    <t>business;scrap;junk;recycling</t>
+  </si>
+  <si>
+    <t>The Organized Mind</t>
+  </si>
+  <si>
+    <t>Daniel Levitin</t>
+  </si>
+  <si>
+    <t>multi-tasking;memory;productivity;self-improvement;thinking;psychology</t>
+  </si>
+  <si>
+    <t>16 Hours 20 Mins</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2633,6 +2654,52 @@
       </c>
       <c r="G61" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>279</v>
+      </c>
+      <c r="B62" t="s">
+        <v>280</v>
+      </c>
+      <c r="C62" s="1">
+        <v>43939</v>
+      </c>
+      <c r="D62" s="1">
+        <v>43946</v>
+      </c>
+      <c r="E62" t="s">
+        <v>281</v>
+      </c>
+      <c r="F62" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" t="s">
+        <v>283</v>
+      </c>
+      <c r="C63" s="1">
+        <v>43945</v>
+      </c>
+      <c r="D63" s="1">
+        <v>43947</v>
+      </c>
+      <c r="E63" t="s">
+        <v>284</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the bullet journal method
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC45CA3-EF45-4F74-84A0-164A37545B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E31BA13-89C3-4C1C-89B4-B306B9B6688F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="306">
   <si>
     <t>Title</t>
   </si>
@@ -938,6 +938,18 @@
   </si>
   <si>
     <t>299 Pages</t>
+  </si>
+  <si>
+    <t>The Bullet Journal Method</t>
+  </si>
+  <si>
+    <t>Ryder Carroll</t>
+  </si>
+  <si>
+    <t>journaling;productivity</t>
+  </si>
+  <si>
+    <t>5 Hours 43 Mins</t>
   </si>
 </sst>
 </file>
@@ -1293,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2840,6 +2852,29 @@
       </c>
       <c r="G67" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>302</v>
+      </c>
+      <c r="B68" t="s">
+        <v>303</v>
+      </c>
+      <c r="C68" s="1">
+        <v>43951</v>
+      </c>
+      <c r="D68" s="1">
+        <v>43952</v>
+      </c>
+      <c r="E68" t="s">
+        <v>304</v>
+      </c>
+      <c r="F68" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the real crash and the story of neuroscience
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E31BA13-89C3-4C1C-89B4-B306B9B6688F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0448D24E-FB26-45A5-993B-1F6D4FEE2EF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="314">
   <si>
     <t>Title</t>
   </si>
@@ -950,6 +950,30 @@
   </si>
   <si>
     <t>5 Hours 43 Mins</t>
+  </si>
+  <si>
+    <t>The Real Crash</t>
+  </si>
+  <si>
+    <t>Peter Schiff</t>
+  </si>
+  <si>
+    <t>economics;national debt;politics;libertarianism;investing</t>
+  </si>
+  <si>
+    <t>12 Hours 55 Mins</t>
+  </si>
+  <si>
+    <t>The Story of Neuroscience</t>
+  </si>
+  <si>
+    <t>Anne Rooney</t>
+  </si>
+  <si>
+    <t>neuroscience;science;brain;history</t>
+  </si>
+  <si>
+    <t>202 Pages</t>
   </si>
 </sst>
 </file>
@@ -1305,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2875,6 +2899,52 @@
       </c>
       <c r="G68" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>306</v>
+      </c>
+      <c r="B69" t="s">
+        <v>307</v>
+      </c>
+      <c r="C69" s="1">
+        <v>43952</v>
+      </c>
+      <c r="D69" s="1">
+        <v>43954</v>
+      </c>
+      <c r="E69" t="s">
+        <v>308</v>
+      </c>
+      <c r="F69" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" t="s">
+        <v>311</v>
+      </c>
+      <c r="C70" s="1">
+        <v>43952</v>
+      </c>
+      <c r="D70" s="1">
+        <v>43955</v>
+      </c>
+      <c r="E70" t="s">
+        <v>312</v>
+      </c>
+      <c r="F70" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added this is chance
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0448D24E-FB26-45A5-993B-1F6D4FEE2EF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9513BC-E955-4FC8-9CC3-E7ECBA51192B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="318">
   <si>
     <t>Title</t>
   </si>
@@ -974,6 +974,18 @@
   </si>
   <si>
     <t>202 Pages</t>
+  </si>
+  <si>
+    <t>This is Chance</t>
+  </si>
+  <si>
+    <t>Jon Mooallen</t>
+  </si>
+  <si>
+    <t>history;alaska;earthquake;radio;leadership</t>
+  </si>
+  <si>
+    <t>8 Hours 27 Mins</t>
   </si>
 </sst>
 </file>
@@ -1329,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2945,6 +2957,29 @@
       </c>
       <c r="G70" t="s">
         <v>313</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>314</v>
+      </c>
+      <c r="B71" t="s">
+        <v>315</v>
+      </c>
+      <c r="C71" s="1">
+        <v>43955</v>
+      </c>
+      <c r="D71" s="1">
+        <v>43956</v>
+      </c>
+      <c r="E71" t="s">
+        <v>316</v>
+      </c>
+      <c r="F71" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added you never forget your first
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EEBEE4-237B-4EF1-ACC7-85A8864AE3F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9991A0-8490-4213-9897-0CF06148E6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="330">
   <si>
     <t>Title</t>
   </si>
@@ -1010,6 +1010,18 @@
   </si>
   <si>
     <t>2 Hours 25 Mins</t>
+  </si>
+  <si>
+    <t>You Never Forget Your First</t>
+  </si>
+  <si>
+    <t>Alexis Coe</t>
+  </si>
+  <si>
+    <t>george washington;history;biography;president;revolutionary war;american history</t>
+  </si>
+  <si>
+    <t>6 Hours 42 Mins</t>
   </si>
 </sst>
 </file>
@@ -1365,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3050,6 +3062,29 @@
       </c>
       <c r="G73" t="s">
         <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>326</v>
+      </c>
+      <c r="B74" t="s">
+        <v>327</v>
+      </c>
+      <c r="C74" s="1">
+        <v>43958</v>
+      </c>
+      <c r="D74" s="1">
+        <v>43959</v>
+      </c>
+      <c r="E74" t="s">
+        <v>328</v>
+      </c>
+      <c r="F74" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added from bacteria to bach and back
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9991A0-8490-4213-9897-0CF06148E6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28464968-7D90-4615-9B0F-C2D4F753A0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="334">
   <si>
     <t>Title</t>
   </si>
@@ -1022,6 +1022,18 @@
   </si>
   <si>
     <t>6 Hours 42 Mins</t>
+  </si>
+  <si>
+    <t>From Bacteria to Bach and Back</t>
+  </si>
+  <si>
+    <t>Daniel C Dennett</t>
+  </si>
+  <si>
+    <t>consciousness;matter;science;neurology;free will</t>
+  </si>
+  <si>
+    <t>15 Hours 52 Mins</t>
   </si>
 </sst>
 </file>
@@ -1377,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3085,6 +3097,29 @@
       </c>
       <c r="G74" t="s">
         <v>329</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>330</v>
+      </c>
+      <c r="B75" t="s">
+        <v>331</v>
+      </c>
+      <c r="C75" s="1">
+        <v>43959</v>
+      </c>
+      <c r="D75" s="1">
+        <v>43962</v>
+      </c>
+      <c r="E75" t="s">
+        <v>332</v>
+      </c>
+      <c r="F75" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added talk like ted and the elephant in the brain
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B14DE0-F9F9-4423-870D-8C1C05ED3228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ABB5D6-2362-4145-9809-51FDC2E96545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="344">
   <si>
     <t>Title</t>
   </si>
@@ -1040,6 +1040,30 @@
   </si>
   <si>
     <t>265 Pages</t>
+  </si>
+  <si>
+    <t>Talk Like Ted</t>
+  </si>
+  <si>
+    <t>Carmine Gallo</t>
+  </si>
+  <si>
+    <t>presentation;speaking;persuasion;presence</t>
+  </si>
+  <si>
+    <t>7 Hours 42 Mins</t>
+  </si>
+  <si>
+    <t>The Elephant in the Brain</t>
+  </si>
+  <si>
+    <t>Kevin Simler</t>
+  </si>
+  <si>
+    <t>psycology;sociology;brain;humans;politics</t>
+  </si>
+  <si>
+    <t>10 Hours 32 Mins</t>
   </si>
 </sst>
 </file>
@@ -1395,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3149,6 +3173,52 @@
       </c>
       <c r="G76" t="s">
         <v>335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>336</v>
+      </c>
+      <c r="B77" t="s">
+        <v>337</v>
+      </c>
+      <c r="C77" s="1">
+        <v>43962</v>
+      </c>
+      <c r="D77" s="1">
+        <v>43965</v>
+      </c>
+      <c r="E77" t="s">
+        <v>338</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>340</v>
+      </c>
+      <c r="B78" t="s">
+        <v>341</v>
+      </c>
+      <c r="C78" s="1">
+        <v>43965</v>
+      </c>
+      <c r="D78" s="1">
+        <v>43970</v>
+      </c>
+      <c r="E78" t="s">
+        <v>342</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sam walton made in america
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0789A116-A06B-46A0-93EC-14A38D2E37A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C5E6D9-E053-45D0-AAFC-0E5939F3EDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="352">
   <si>
     <t>Title</t>
   </si>
@@ -1076,6 +1078,18 @@
   </si>
   <si>
     <t>10 Hours 56 Mins</t>
+  </si>
+  <si>
+    <t>Sam Walton, Made in America</t>
+  </si>
+  <si>
+    <t>Sam Walton</t>
+  </si>
+  <si>
+    <t>biography;sam walton;business;walmart;retail</t>
+  </si>
+  <si>
+    <t>379 Pages</t>
   </si>
 </sst>
 </file>
@@ -1431,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3254,6 +3268,29 @@
       </c>
       <c r="G79" t="s">
         <v>347</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>348</v>
+      </c>
+      <c r="B80" t="s">
+        <v>349</v>
+      </c>
+      <c r="C80" s="1">
+        <v>43964</v>
+      </c>
+      <c r="D80" s="1">
+        <v>43978</v>
+      </c>
+      <c r="E80" t="s">
+        <v>350</v>
+      </c>
+      <c r="F80" t="s">
+        <v>141</v>
+      </c>
+      <c r="G80" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the vaccine race
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C5E6D9-E053-45D0-AAFC-0E5939F3EDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44408B1C-9118-49E6-85ED-928DCCE7B4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="356">
   <si>
     <t>Title</t>
   </si>
@@ -1090,6 +1090,18 @@
   </si>
   <si>
     <t>379 Pages</t>
+  </si>
+  <si>
+    <t>The Vaccine Race</t>
+  </si>
+  <si>
+    <t>Meredith Wadman</t>
+  </si>
+  <si>
+    <t>vaccines;science;medicine;disease;virus;history</t>
+  </si>
+  <si>
+    <t>19 Hours 19 Mins</t>
   </si>
 </sst>
 </file>
@@ -1445,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3291,6 +3303,29 @@
       </c>
       <c r="G80" t="s">
         <v>351</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>352</v>
+      </c>
+      <c r="B81" t="s">
+        <v>353</v>
+      </c>
+      <c r="C81" s="1">
+        <v>43973</v>
+      </c>
+      <c r="D81" s="1">
+        <v>43979</v>
+      </c>
+      <c r="E81" t="s">
+        <v>354</v>
+      </c>
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the case against socialism
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44408B1C-9118-49E6-85ED-928DCCE7B4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6C141F-BA8F-4898-A6C3-0E6B7BCDDBC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="360">
   <si>
     <t>Title</t>
   </si>
@@ -1102,6 +1102,18 @@
   </si>
   <si>
     <t>19 Hours 19 Mins</t>
+  </si>
+  <si>
+    <t>The Case Against Socialism</t>
+  </si>
+  <si>
+    <t>Rand Paul</t>
+  </si>
+  <si>
+    <t>socialism;politics;economics;capitalism</t>
+  </si>
+  <si>
+    <t>10 Hours 19 Mins</t>
   </si>
 </sst>
 </file>
@@ -1457,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3326,6 +3338,29 @@
       </c>
       <c r="G81" t="s">
         <v>355</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82" t="s">
+        <v>357</v>
+      </c>
+      <c r="C82" s="1">
+        <v>43980</v>
+      </c>
+      <c r="D82" s="1">
+        <v>43983</v>
+      </c>
+      <c r="E82" t="s">
+        <v>358</v>
+      </c>
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added springfield confidential and the years that matter most
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6C141F-BA8F-4898-A6C3-0E6B7BCDDBC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF861B5-7892-4C3A-94DE-DE733D77D2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="367">
   <si>
     <t>Title</t>
   </si>
@@ -1114,6 +1114,27 @@
   </si>
   <si>
     <t>10 Hours 19 Mins</t>
+  </si>
+  <si>
+    <t>The Years That Matter Most</t>
+  </si>
+  <si>
+    <t>Paul Tough</t>
+  </si>
+  <si>
+    <t>college;SAT;admissions;discrimination;equality</t>
+  </si>
+  <si>
+    <t>12 Hours 39 Mins</t>
+  </si>
+  <si>
+    <t>Springfield Confidential</t>
+  </si>
+  <si>
+    <t>Mike Reiss</t>
+  </si>
+  <si>
+    <t>simpsons;tv;writing;comedy;sitcoms</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3361,6 +3382,52 @@
       </c>
       <c r="G82" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" t="s">
+        <v>361</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43984</v>
+      </c>
+      <c r="D83" s="1">
+        <v>43986</v>
+      </c>
+      <c r="E83" t="s">
+        <v>362</v>
+      </c>
+      <c r="F83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>364</v>
+      </c>
+      <c r="B84" t="s">
+        <v>365</v>
+      </c>
+      <c r="C84" s="1">
+        <v>43986</v>
+      </c>
+      <c r="D84" s="1">
+        <v>43987</v>
+      </c>
+      <c r="E84" t="s">
+        <v>366</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added when the air hits your brain
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF861B5-7892-4C3A-94DE-DE733D77D2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66EA68B-CF79-49AC-B713-0E0629A211DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="371">
   <si>
     <t>Title</t>
   </si>
@@ -1135,6 +1135,18 @@
   </si>
   <si>
     <t>simpsons;tv;writing;comedy;sitcoms</t>
+  </si>
+  <si>
+    <t>When The Air Hits Your Brain</t>
+  </si>
+  <si>
+    <t>Frank Vertosick</t>
+  </si>
+  <si>
+    <t>medicine;neurology;neuro surgery;surgery;doctor;residency</t>
+  </si>
+  <si>
+    <t>8 Hours 43 Mins</t>
   </si>
 </sst>
 </file>
@@ -1490,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3428,6 +3440,29 @@
       </c>
       <c r="G84" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>367</v>
+      </c>
+      <c r="B85" t="s">
+        <v>368</v>
+      </c>
+      <c r="C85" s="1">
+        <v>43988</v>
+      </c>
+      <c r="D85" s="1">
+        <v>43990</v>
+      </c>
+      <c r="E85" t="s">
+        <v>369</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added coffeeland, brick by brick, and the virgin way
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C1F2D2-8A1C-4436-99B3-068F194A3368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A74F319-7579-4726-8517-B57716259DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="392">
   <si>
     <t>Title</t>
   </si>
@@ -1171,6 +1171,45 @@
   </si>
   <si>
     <t>23 Hours 25 Mins</t>
+  </si>
+  <si>
+    <t>Coffeeland</t>
+  </si>
+  <si>
+    <t>Augustine Sedgewick</t>
+  </si>
+  <si>
+    <t>coffee;business;socialism;capitalism;exploitation;history</t>
+  </si>
+  <si>
+    <t>15 Hours 2 Mins</t>
+  </si>
+  <si>
+    <t>Brick by Brick</t>
+  </si>
+  <si>
+    <t>David Robertson</t>
+  </si>
+  <si>
+    <t>6/12/20202</t>
+  </si>
+  <si>
+    <t>Lego;business;history;innovation;toys</t>
+  </si>
+  <si>
+    <t>10 Hours 24 Mins</t>
+  </si>
+  <si>
+    <t>The Virgin Way</t>
+  </si>
+  <si>
+    <t>Richard Branson</t>
+  </si>
+  <si>
+    <t>richard branson;business;leadership;virgin;airlines</t>
+  </si>
+  <si>
+    <t>11 Hours 30 Mins</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3533,6 +3572,75 @@
       </c>
       <c r="G87" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>379</v>
+      </c>
+      <c r="B88" t="s">
+        <v>380</v>
+      </c>
+      <c r="C88" s="1">
+        <v>43992</v>
+      </c>
+      <c r="D88" s="1">
+        <v>43994</v>
+      </c>
+      <c r="E88" t="s">
+        <v>381</v>
+      </c>
+      <c r="F88" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>383</v>
+      </c>
+      <c r="B89" t="s">
+        <v>384</v>
+      </c>
+      <c r="C89" t="s">
+        <v>385</v>
+      </c>
+      <c r="D89" s="1">
+        <v>43996</v>
+      </c>
+      <c r="E89" t="s">
+        <v>386</v>
+      </c>
+      <c r="F89" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>388</v>
+      </c>
+      <c r="B90" t="s">
+        <v>389</v>
+      </c>
+      <c r="C90" s="1">
+        <v>43997</v>
+      </c>
+      <c r="D90" s="1">
+        <v>43998</v>
+      </c>
+      <c r="E90" t="s">
+        <v>390</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the magic of thinking big
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A74F319-7579-4726-8517-B57716259DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1925D1-F26E-431B-AA7E-47D610E6C4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="396">
   <si>
     <t>Title</t>
   </si>
@@ -1210,6 +1210,18 @@
   </si>
   <si>
     <t>11 Hours 30 Mins</t>
+  </si>
+  <si>
+    <t>The Magic of Thinking Big</t>
+  </si>
+  <si>
+    <t>David Schwartz</t>
+  </si>
+  <si>
+    <t>confidence;self-improvement;goals;positivity</t>
+  </si>
+  <si>
+    <t>9 Hours 31 Mins</t>
   </si>
 </sst>
 </file>
@@ -1565,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3641,6 +3653,29 @@
       </c>
       <c r="G90" t="s">
         <v>391</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>392</v>
+      </c>
+      <c r="B91" t="s">
+        <v>393</v>
+      </c>
+      <c r="C91" s="1">
+        <v>43998</v>
+      </c>
+      <c r="D91" s="1">
+        <v>44000</v>
+      </c>
+      <c r="E91" t="s">
+        <v>394</v>
+      </c>
+      <c r="F91" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added multipliers and an economist walks into a brothel
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1925D1-F26E-431B-AA7E-47D610E6C4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF536935-83A2-4171-9D50-3D4809CC312B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="404">
   <si>
     <t>Title</t>
   </si>
@@ -1222,6 +1222,30 @@
   </si>
   <si>
     <t>9 Hours 31 Mins</t>
+  </si>
+  <si>
+    <t>Multipliers</t>
+  </si>
+  <si>
+    <t>Liz Wiseman</t>
+  </si>
+  <si>
+    <t>leadership;growth mindset;development</t>
+  </si>
+  <si>
+    <t>7 Hours 53 Mins</t>
+  </si>
+  <si>
+    <t>An Economist Walks Into a Brothel</t>
+  </si>
+  <si>
+    <t>Allison Schrager</t>
+  </si>
+  <si>
+    <t>economics;risk;risk management;</t>
+  </si>
+  <si>
+    <t>7 Hours 38 Mins</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3676,6 +3700,52 @@
       </c>
       <c r="G91" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>396</v>
+      </c>
+      <c r="B92" t="s">
+        <v>397</v>
+      </c>
+      <c r="C92" s="1">
+        <v>44000</v>
+      </c>
+      <c r="D92" s="1">
+        <v>44003</v>
+      </c>
+      <c r="E92" t="s">
+        <v>398</v>
+      </c>
+      <c r="F92" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>400</v>
+      </c>
+      <c r="B93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C93" s="1">
+        <v>44003</v>
+      </c>
+      <c r="D93" s="1">
+        <v>44004</v>
+      </c>
+      <c r="E93" t="s">
+        <v>402</v>
+      </c>
+      <c r="F93" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a wizard of earthsea and best movie year ever
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396FC6B4-F4EA-4C4C-A359-F4D198573FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853653A6-9B17-4007-A0E3-2A6C5C6F5499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Books I want to read" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="419">
   <si>
     <t>Title</t>
   </si>
@@ -1280,6 +1279,18 @@
   </si>
   <si>
     <t>14 Hours 20 Mins</t>
+  </si>
+  <si>
+    <t>A Wizard of Earthsea</t>
+  </si>
+  <si>
+    <t>Ursula K Le Guin</t>
+  </si>
+  <si>
+    <t>fiction;wizard;fantasy;quest</t>
+  </si>
+  <si>
+    <t>145 Pages</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3815,6 +3826,9 @@
       <c r="C95" s="1">
         <v>44005</v>
       </c>
+      <c r="D95" s="1">
+        <v>44011</v>
+      </c>
       <c r="E95" t="s">
         <v>410</v>
       </c>
@@ -3846,6 +3860,29 @@
       </c>
       <c r="G96" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>415</v>
+      </c>
+      <c r="B97" t="s">
+        <v>416</v>
+      </c>
+      <c r="C97" s="1">
+        <v>44011</v>
+      </c>
+      <c r="D97" s="1">
+        <v>44012</v>
+      </c>
+      <c r="E97" t="s">
+        <v>417</v>
+      </c>
+      <c r="F97" t="s">
+        <v>17</v>
+      </c>
+      <c r="G97" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added how emotions are made
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853653A6-9B17-4007-A0E3-2A6C5C6F5499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B543BD-E02B-42D1-A9F8-B3AF4A8B968D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="423">
   <si>
     <t>Title</t>
   </si>
@@ -1291,6 +1291,18 @@
   </si>
   <si>
     <t>145 Pages</t>
+  </si>
+  <si>
+    <t>How Emotions are Made</t>
+  </si>
+  <si>
+    <t>Lisa Feldman Barrett</t>
+  </si>
+  <si>
+    <t>emotion;psychology;perception;Charles Darwin;science</t>
+  </si>
+  <si>
+    <t>14 Hours 32 Mins</t>
   </si>
 </sst>
 </file>
@@ -1646,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3883,6 +3895,29 @@
       </c>
       <c r="G97" t="s">
         <v>418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>419</v>
+      </c>
+      <c r="B98" t="s">
+        <v>420</v>
+      </c>
+      <c r="C98" s="1">
+        <v>44011</v>
+      </c>
+      <c r="D98" s="1">
+        <v>44013</v>
+      </c>
+      <c r="E98" t="s">
+        <v>421</v>
+      </c>
+      <c r="F98" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the tombs of atuan
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B543BD-E02B-42D1-A9F8-B3AF4A8B968D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB945A44-44D3-44E8-B107-B410E244E4F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="426">
   <si>
     <t>Title</t>
   </si>
@@ -1303,6 +1303,15 @@
   </si>
   <si>
     <t>14 Hours 32 Mins</t>
+  </si>
+  <si>
+    <t>The Tombs of Atuan</t>
+  </si>
+  <si>
+    <t>wizards;fiction;earthsea;magic;fantasy</t>
+  </si>
+  <si>
+    <t>117 Pages</t>
   </si>
 </sst>
 </file>
@@ -1658,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3918,6 +3927,29 @@
       </c>
       <c r="G98" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>423</v>
+      </c>
+      <c r="B99" t="s">
+        <v>416</v>
+      </c>
+      <c r="C99" s="1">
+        <v>44013</v>
+      </c>
+      <c r="D99" s="1">
+        <v>44013</v>
+      </c>
+      <c r="E99" t="s">
+        <v>424</v>
+      </c>
+      <c r="F99" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the hidden life of trees
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB945A44-44D3-44E8-B107-B410E244E4F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB3DFE6-0B3C-458E-84B7-69A1F05749A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="430">
   <si>
     <t>Title</t>
   </si>
@@ -1312,6 +1312,18 @@
   </si>
   <si>
     <t>117 Pages</t>
+  </si>
+  <si>
+    <t>The Hidden Life of Trees</t>
+  </si>
+  <si>
+    <t>Peter Wohlleben</t>
+  </si>
+  <si>
+    <t>trees;science;life;biology;chlorophyll;forests</t>
+  </si>
+  <si>
+    <t>7 Hours 33 Mins</t>
   </si>
 </sst>
 </file>
@@ -1667,10 +1679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3950,6 +3962,29 @@
       </c>
       <c r="G99" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>426</v>
+      </c>
+      <c r="B100" t="s">
+        <v>427</v>
+      </c>
+      <c r="C100" s="1">
+        <v>44014</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44016</v>
+      </c>
+      <c r="E100" t="s">
+        <v>428</v>
+      </c>
+      <c r="F100" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the farthest shore
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811308B4-F699-48D1-8405-C3D0AA1DC277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF77AF4-1276-4035-B154-38B58FD53169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="437">
   <si>
     <t>Title</t>
   </si>
@@ -1336,6 +1336,15 @@
   </si>
   <si>
     <t>4 Hours 51 Mins</t>
+  </si>
+  <si>
+    <t>The Farthest Shore</t>
+  </si>
+  <si>
+    <t>fantasy;wizards;earthsea;ged;quest;magic;sorcery</t>
+  </si>
+  <si>
+    <t>155 Pages</t>
   </si>
 </sst>
 </file>
@@ -1691,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4020,6 +4029,29 @@
       </c>
       <c r="G101" t="s">
         <v>433</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>434</v>
+      </c>
+      <c r="B102" t="s">
+        <v>416</v>
+      </c>
+      <c r="C102" s="1">
+        <v>44014</v>
+      </c>
+      <c r="D102" s="1">
+        <v>44017</v>
+      </c>
+      <c r="E102" t="s">
+        <v>435</v>
+      </c>
+      <c r="F102" t="s">
+        <v>17</v>
+      </c>
+      <c r="G102" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the big short and what the most successful people do at work
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FAF5C2-3765-4E57-AA11-0A98BA8C1D21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5049483B-DAD0-4412-A3EC-0EC9ABBCE3B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="448">
   <si>
     <t>Title</t>
   </si>
@@ -1357,6 +1357,27 @@
   </si>
   <si>
     <t>10 Hours 16 Mins</t>
+  </si>
+  <si>
+    <t>The Big Short</t>
+  </si>
+  <si>
+    <t>bonds;mortgage backed securities;shorting;wall street;finance;financial crisis</t>
+  </si>
+  <si>
+    <t>9 Hours 30 Mins</t>
+  </si>
+  <si>
+    <t>What the Most Successful People Do At Work</t>
+  </si>
+  <si>
+    <t>Laura Vanderkam</t>
+  </si>
+  <si>
+    <t>success;time management;planning;career;self-improvement</t>
+  </si>
+  <si>
+    <t>2 Hours 4 Mins</t>
   </si>
 </sst>
 </file>
@@ -1712,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4087,6 +4108,52 @@
       </c>
       <c r="G103" t="s">
         <v>440</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>441</v>
+      </c>
+      <c r="B104" t="s">
+        <v>438</v>
+      </c>
+      <c r="C104" s="1">
+        <v>44018</v>
+      </c>
+      <c r="D104" s="1">
+        <v>44019</v>
+      </c>
+      <c r="E104" t="s">
+        <v>442</v>
+      </c>
+      <c r="F104" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>444</v>
+      </c>
+      <c r="B105" t="s">
+        <v>445</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44019</v>
+      </c>
+      <c r="D105" s="1">
+        <v>44019</v>
+      </c>
+      <c r="E105" t="s">
+        <v>446</v>
+      </c>
+      <c r="F105" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ratings for each book read
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BCF5A6-12A0-41F7-A21D-3D45D2857B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3BFE42-F035-4E6F-9871-7F8AAAE93C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="458">
   <si>
     <t>Title</t>
   </si>
@@ -1764,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1907,6 +1907,9 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1930,6 +1933,9 @@
       <c r="G6" t="s">
         <v>28</v>
       </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1953,6 +1959,9 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1976,6 +1985,9 @@
       <c r="G8" t="s">
         <v>36</v>
       </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1999,6 +2011,9 @@
       <c r="G9" t="s">
         <v>80</v>
       </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -2022,6 +2037,9 @@
       <c r="G10" t="s">
         <v>84</v>
       </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -2045,6 +2063,9 @@
       <c r="G11" t="s">
         <v>88</v>
       </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -2068,6 +2089,9 @@
       <c r="G12" t="s">
         <v>92</v>
       </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -2091,6 +2115,9 @@
       <c r="G13" t="s">
         <v>95</v>
       </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -2114,6 +2141,9 @@
       <c r="G14" t="s">
         <v>107</v>
       </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -2137,6 +2167,9 @@
       <c r="G15" t="s">
         <v>106</v>
       </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -2160,8 +2193,11 @@
       <c r="G16" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -2183,8 +2219,11 @@
       <c r="G17" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2206,8 +2245,11 @@
       <c r="G18" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2229,8 +2271,11 @@
       <c r="G19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2252,8 +2297,11 @@
       <c r="G20" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2275,8 +2323,11 @@
       <c r="G21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2298,8 +2349,11 @@
       <c r="G22" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -2321,8 +2375,11 @@
       <c r="G23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -2344,602 +2401,692 @@
       <c r="G24" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
       </c>
       <c r="C25" s="1">
-        <v>43874</v>
+        <v>43876</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43878</v>
       </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1">
-        <v>43876</v>
+        <v>43879</v>
       </c>
       <c r="D26" s="1">
-        <v>43878</v>
+        <v>43879</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C27" s="1">
         <v>43879</v>
       </c>
       <c r="D27" s="1">
-        <v>43879</v>
+        <v>43880</v>
       </c>
       <c r="E27" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1">
-        <v>43879</v>
+        <v>43867</v>
       </c>
       <c r="D28" s="1">
         <v>43880</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="C29" s="1">
-        <v>43867</v>
+        <v>43881</v>
       </c>
       <c r="D29" s="1">
-        <v>43880</v>
+        <v>43888</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1">
-        <v>43881</v>
+        <v>43888</v>
       </c>
       <c r="D30" s="1">
         <v>43888</v>
       </c>
       <c r="E30" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C31" s="1">
         <v>43888</v>
       </c>
       <c r="D31" s="1">
-        <v>43888</v>
+        <v>43889</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1">
-        <v>43888</v>
+        <v>43889</v>
       </c>
       <c r="D32" s="1">
-        <v>43889</v>
+        <v>43892</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C33" s="1">
-        <v>43889</v>
+        <v>43892</v>
       </c>
       <c r="D33" s="1">
-        <v>43892</v>
+        <v>43895</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
       </c>
       <c r="G33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C34" s="1">
-        <v>43892</v>
+        <v>43881</v>
       </c>
       <c r="D34" s="1">
+        <v>43897</v>
+      </c>
+      <c r="E34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="1">
         <v>43895</v>
-      </c>
-      <c r="E34" t="s">
-        <v>176</v>
-      </c>
-      <c r="F34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" t="s">
-        <v>178</v>
-      </c>
-      <c r="C35" s="1">
-        <v>43881</v>
       </c>
       <c r="D35" s="1">
         <v>43897</v>
       </c>
       <c r="E35" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>184</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="1">
+        <v>43901</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43902</v>
+      </c>
+      <c r="E36" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>188</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" s="1">
+        <v>43904</v>
+      </c>
+      <c r="D37" s="1">
+        <v>43906</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>191</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>192</v>
+      </c>
+      <c r="B38" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="1">
+        <v>43907</v>
+      </c>
+      <c r="D38" s="1">
+        <v>43910</v>
+      </c>
+      <c r="E38" t="s">
+        <v>194</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>175</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" s="1">
+        <v>43898</v>
+      </c>
+      <c r="D39" s="1">
+        <v>43911</v>
+      </c>
+      <c r="E39" t="s">
+        <v>197</v>
+      </c>
+      <c r="F39" t="s">
         <v>17</v>
       </c>
-      <c r="G35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="1">
-        <v>43895</v>
-      </c>
-      <c r="D36" s="1">
-        <v>43897</v>
-      </c>
-      <c r="E36" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>185</v>
-      </c>
-      <c r="B37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" s="1">
-        <v>43901</v>
-      </c>
-      <c r="D37" s="1">
-        <v>43902</v>
-      </c>
-      <c r="E37" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" t="s">
-        <v>190</v>
-      </c>
-      <c r="C38" s="1">
-        <v>43904</v>
-      </c>
-      <c r="D38" s="1">
-        <v>43906</v>
-      </c>
-      <c r="E38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B39" t="s">
-        <v>193</v>
-      </c>
-      <c r="C39" s="1">
-        <v>43907</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="G39" t="s">
+        <v>198</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="1">
         <v>43910</v>
       </c>
-      <c r="E39" t="s">
-        <v>194</v>
-      </c>
-      <c r="F39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>195</v>
-      </c>
-      <c r="B40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C40" s="1">
-        <v>43898</v>
-      </c>
       <c r="D40" s="1">
-        <v>43911</v>
+        <v>43912</v>
       </c>
       <c r="E40" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C41" s="1">
-        <v>43910</v>
+        <v>43912</v>
       </c>
       <c r="D41" s="1">
         <v>43912</v>
       </c>
       <c r="E41" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F41" t="s">
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B42" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C42" s="1">
         <v>43912</v>
       </c>
       <c r="D42" s="1">
-        <v>43912</v>
+        <v>43913</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C43" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="D43" s="1">
         <v>43913</v>
       </c>
       <c r="E43" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G43" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="B44" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C44" s="1">
-        <v>43911</v>
+        <v>43913</v>
       </c>
       <c r="D44" s="1">
-        <v>43913</v>
+        <v>43918</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="F44" t="s">
         <v>17</v>
       </c>
       <c r="G44" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C45" s="1">
         <v>43913</v>
       </c>
       <c r="D45" s="1">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C46" s="1">
-        <v>43913</v>
+        <v>43919</v>
       </c>
       <c r="D46" s="1">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="E46" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B47" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C47" s="1">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D47" s="1">
         <v>43920</v>
       </c>
       <c r="E47" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
       </c>
       <c r="G47" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B48" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C48" s="1">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D48" s="1">
-        <v>43920</v>
+        <v>43922</v>
       </c>
       <c r="E48" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B49" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C49" s="1">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D49" s="1">
-        <v>43922</v>
+        <v>43927</v>
       </c>
       <c r="E49" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C50" s="1">
-        <v>43922</v>
+        <v>43927</v>
       </c>
       <c r="D50" s="1">
-        <v>43927</v>
+        <v>43930</v>
       </c>
       <c r="E50" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G50" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B51" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C51" s="1">
         <v>43927</v>
@@ -2948,1255 +3095,1394 @@
         <v>43930</v>
       </c>
       <c r="E51" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>243</v>
+      </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" t="s">
+        <v>245</v>
+      </c>
+      <c r="C52" s="1">
+        <v>43930</v>
+      </c>
+      <c r="D52" s="1">
+        <v>43934</v>
+      </c>
+      <c r="E52" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>247</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>248</v>
+      </c>
+      <c r="B53" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" s="1">
+        <v>43931</v>
+      </c>
+      <c r="D53" s="1">
+        <v>43936</v>
+      </c>
+      <c r="E53" t="s">
+        <v>250</v>
+      </c>
+      <c r="F53" t="s">
         <v>17</v>
       </c>
-      <c r="G51" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>240</v>
-      </c>
-      <c r="B52" t="s">
-        <v>241</v>
-      </c>
-      <c r="C52" s="1">
-        <v>43927</v>
-      </c>
-      <c r="D52" s="1">
-        <v>43930</v>
-      </c>
-      <c r="E52" t="s">
-        <v>242</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>244</v>
-      </c>
-      <c r="B53" t="s">
-        <v>245</v>
-      </c>
-      <c r="C53" s="1">
-        <v>43930</v>
-      </c>
-      <c r="D53" s="1">
-        <v>43934</v>
-      </c>
-      <c r="E53" t="s">
-        <v>246</v>
-      </c>
-      <c r="F53" t="s">
-        <v>16</v>
-      </c>
       <c r="G53" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C54" s="1">
-        <v>43931</v>
+        <v>43937</v>
       </c>
       <c r="D54" s="1">
-        <v>43936</v>
+        <v>43938</v>
       </c>
       <c r="E54" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F54" t="s">
         <v>17</v>
       </c>
       <c r="G54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C55" s="1">
-        <v>43937</v>
+        <v>43935</v>
       </c>
       <c r="D55" s="1">
-        <v>43938</v>
+        <v>43939</v>
       </c>
       <c r="E55" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B56" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C56" s="1">
-        <v>43935</v>
+        <v>43939</v>
       </c>
       <c r="D56" s="1">
-        <v>43939</v>
+        <v>43940</v>
       </c>
       <c r="E56" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
       </c>
       <c r="G56" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B57" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="C57" s="1">
-        <v>43939</v>
+        <v>43940</v>
       </c>
       <c r="D57" s="1">
         <v>43940</v>
       </c>
       <c r="E57" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F57" t="s">
         <v>16</v>
       </c>
       <c r="G57" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>268</v>
       </c>
       <c r="C58" s="1">
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="D58" s="1">
-        <v>43940</v>
+        <v>43942</v>
       </c>
       <c r="E58" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="F58" t="s">
         <v>16</v>
       </c>
       <c r="G58" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B59" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C59" s="1">
-        <v>43941</v>
+        <v>43942</v>
       </c>
       <c r="D59" s="1">
         <v>43942</v>
       </c>
       <c r="E59" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
       </c>
       <c r="G59" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B60" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C60" s="1">
         <v>43942</v>
       </c>
       <c r="D60" s="1">
-        <v>43942</v>
+        <v>43944</v>
       </c>
       <c r="E60" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="F60" t="s">
         <v>16</v>
       </c>
       <c r="G60" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+      <c r="H60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B61" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C61" s="1">
-        <v>43942</v>
+        <v>43939</v>
       </c>
       <c r="D61" s="1">
-        <v>43944</v>
+        <v>43946</v>
       </c>
       <c r="E61" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="G61" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="H61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B62" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C62" s="1">
-        <v>43939</v>
+        <v>43945</v>
       </c>
       <c r="D62" s="1">
-        <v>43946</v>
+        <v>43947</v>
       </c>
       <c r="E62" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F62" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="G62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+      <c r="H62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B63" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C63" s="1">
-        <v>43945</v>
+        <v>43836</v>
       </c>
       <c r="D63" s="1">
         <v>43947</v>
       </c>
       <c r="E63" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G63" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+      <c r="H63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B64" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C64" s="1">
-        <v>43836</v>
+        <v>43947</v>
       </c>
       <c r="D64" s="1">
+        <v>43948</v>
+      </c>
+      <c r="E64" t="s">
+        <v>292</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" t="s">
+        <v>293</v>
+      </c>
+      <c r="H64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>294</v>
+      </c>
+      <c r="B65" t="s">
+        <v>295</v>
+      </c>
+      <c r="C65" s="1">
+        <v>43948</v>
+      </c>
+      <c r="D65" s="1">
+        <v>43951</v>
+      </c>
+      <c r="E65" t="s">
+        <v>296</v>
+      </c>
+      <c r="F65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>297</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>298</v>
+      </c>
+      <c r="B66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" s="1">
         <v>43947</v>
-      </c>
-      <c r="E64" t="s">
-        <v>288</v>
-      </c>
-      <c r="F64" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>290</v>
-      </c>
-      <c r="B65" t="s">
-        <v>291</v>
-      </c>
-      <c r="C65" s="1">
-        <v>43947</v>
-      </c>
-      <c r="D65" s="1">
-        <v>43948</v>
-      </c>
-      <c r="E65" t="s">
-        <v>292</v>
-      </c>
-      <c r="F65" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>294</v>
-      </c>
-      <c r="B66" t="s">
-        <v>295</v>
-      </c>
-      <c r="C66" s="1">
-        <v>43948</v>
       </c>
       <c r="D66" s="1">
         <v>43951</v>
       </c>
       <c r="E66" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G66" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+      <c r="H66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B67" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C67" s="1">
-        <v>43947</v>
+        <v>43951</v>
       </c>
       <c r="D67" s="1">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="E67" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G67" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+      <c r="H67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C68" s="1">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="D68" s="1">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="E68" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F68" t="s">
         <v>16</v>
       </c>
       <c r="G68" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B69" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C69" s="1">
         <v>43952</v>
       </c>
       <c r="D69" s="1">
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="E69" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G69" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B70" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C70" s="1">
-        <v>43952</v>
+        <v>43955</v>
       </c>
       <c r="D70" s="1">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="E70" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G70" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B71" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C71" s="1">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D71" s="1">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="E71" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F71" t="s">
         <v>16</v>
       </c>
       <c r="G71" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+      <c r="H71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B72" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C72" s="1">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D72" s="1">
         <v>43958</v>
       </c>
       <c r="E72" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="F72" t="s">
         <v>16</v>
       </c>
       <c r="G72" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+      <c r="H72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B73" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C73" s="1">
         <v>43958</v>
       </c>
       <c r="D73" s="1">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="E73" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
       </c>
       <c r="G73" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="H73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B74" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C74" s="1">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D74" s="1">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="E74" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
       </c>
       <c r="G74" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+      <c r="H74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>330</v>
+        <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>331</v>
+        <v>43</v>
       </c>
       <c r="C75" s="1">
-        <v>43959</v>
+        <v>43956</v>
       </c>
       <c r="D75" s="1">
+        <v>43963</v>
+      </c>
+      <c r="E75" t="s">
+        <v>334</v>
+      </c>
+      <c r="F75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75" t="s">
+        <v>335</v>
+      </c>
+      <c r="H75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" t="s">
+        <v>337</v>
+      </c>
+      <c r="C76" s="1">
         <v>43962</v>
       </c>
-      <c r="E75" t="s">
-        <v>332</v>
-      </c>
-      <c r="F75" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>42</v>
-      </c>
-      <c r="B76" t="s">
-        <v>43</v>
-      </c>
-      <c r="C76" s="1">
-        <v>43956</v>
-      </c>
       <c r="D76" s="1">
-        <v>43963</v>
+        <v>43965</v>
       </c>
       <c r="E76" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="F76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" t="s">
+        <v>339</v>
+      </c>
+      <c r="H76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" t="s">
+        <v>341</v>
+      </c>
+      <c r="C77" s="1">
+        <v>43965</v>
+      </c>
+      <c r="D77" s="1">
+        <v>43970</v>
+      </c>
+      <c r="E77" t="s">
+        <v>342</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>343</v>
+      </c>
+      <c r="H77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>344</v>
+      </c>
+      <c r="B78" t="s">
+        <v>345</v>
+      </c>
+      <c r="C78" s="1">
+        <v>43970</v>
+      </c>
+      <c r="D78" s="1">
+        <v>43972</v>
+      </c>
+      <c r="E78" t="s">
+        <v>346</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
+        <v>347</v>
+      </c>
+      <c r="H78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>348</v>
+      </c>
+      <c r="B79" t="s">
+        <v>349</v>
+      </c>
+      <c r="C79" s="1">
+        <v>43964</v>
+      </c>
+      <c r="D79" s="1">
+        <v>43978</v>
+      </c>
+      <c r="E79" t="s">
+        <v>350</v>
+      </c>
+      <c r="F79" t="s">
+        <v>141</v>
+      </c>
+      <c r="G79" t="s">
+        <v>351</v>
+      </c>
+      <c r="H79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>352</v>
+      </c>
+      <c r="B80" t="s">
+        <v>353</v>
+      </c>
+      <c r="C80" s="1">
+        <v>43973</v>
+      </c>
+      <c r="D80" s="1">
+        <v>43979</v>
+      </c>
+      <c r="E80" t="s">
+        <v>354</v>
+      </c>
+      <c r="F80" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" t="s">
+        <v>355</v>
+      </c>
+      <c r="H80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>356</v>
+      </c>
+      <c r="B81" t="s">
+        <v>357</v>
+      </c>
+      <c r="C81" s="1">
+        <v>43980</v>
+      </c>
+      <c r="D81" s="1">
+        <v>43983</v>
+      </c>
+      <c r="E81" t="s">
+        <v>358</v>
+      </c>
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" t="s">
+        <v>359</v>
+      </c>
+      <c r="H81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>360</v>
+      </c>
+      <c r="B82" t="s">
+        <v>361</v>
+      </c>
+      <c r="C82" s="1">
+        <v>43984</v>
+      </c>
+      <c r="D82" s="1">
+        <v>43986</v>
+      </c>
+      <c r="E82" t="s">
+        <v>362</v>
+      </c>
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>363</v>
+      </c>
+      <c r="H82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>364</v>
+      </c>
+      <c r="B83" t="s">
+        <v>365</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43986</v>
+      </c>
+      <c r="D83" s="1">
+        <v>43987</v>
+      </c>
+      <c r="E83" t="s">
+        <v>366</v>
+      </c>
+      <c r="F83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>293</v>
+      </c>
+      <c r="H83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>367</v>
+      </c>
+      <c r="B84" t="s">
+        <v>368</v>
+      </c>
+      <c r="C84" s="1">
+        <v>43988</v>
+      </c>
+      <c r="D84" s="1">
+        <v>43990</v>
+      </c>
+      <c r="E84" t="s">
+        <v>369</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>370</v>
+      </c>
+      <c r="H84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>371</v>
+      </c>
+      <c r="B85" t="s">
+        <v>372</v>
+      </c>
+      <c r="C85" s="1">
+        <v>43979</v>
+      </c>
+      <c r="D85" s="1">
+        <v>43991</v>
+      </c>
+      <c r="E85" t="s">
+        <v>373</v>
+      </c>
+      <c r="F85" t="s">
         <v>17</v>
       </c>
-      <c r="G76" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>336</v>
-      </c>
-      <c r="B77" t="s">
-        <v>337</v>
-      </c>
-      <c r="C77" s="1">
-        <v>43962</v>
-      </c>
-      <c r="D77" s="1">
-        <v>43965</v>
-      </c>
-      <c r="E77" t="s">
-        <v>338</v>
-      </c>
-      <c r="F77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>340</v>
-      </c>
-      <c r="B78" t="s">
-        <v>341</v>
-      </c>
-      <c r="C78" s="1">
-        <v>43965</v>
-      </c>
-      <c r="D78" s="1">
-        <v>43970</v>
-      </c>
-      <c r="E78" t="s">
-        <v>342</v>
-      </c>
-      <c r="F78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>344</v>
-      </c>
-      <c r="B79" t="s">
-        <v>345</v>
-      </c>
-      <c r="C79" s="1">
-        <v>43970</v>
-      </c>
-      <c r="D79" s="1">
-        <v>43972</v>
-      </c>
-      <c r="E79" t="s">
-        <v>346</v>
-      </c>
-      <c r="F79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>348</v>
-      </c>
-      <c r="B80" t="s">
-        <v>349</v>
-      </c>
-      <c r="C80" s="1">
-        <v>43964</v>
-      </c>
-      <c r="D80" s="1">
-        <v>43978</v>
-      </c>
-      <c r="E80" t="s">
-        <v>350</v>
-      </c>
-      <c r="F80" t="s">
-        <v>141</v>
-      </c>
-      <c r="G80" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>352</v>
-      </c>
-      <c r="B81" t="s">
-        <v>353</v>
-      </c>
-      <c r="C81" s="1">
-        <v>43973</v>
-      </c>
-      <c r="D81" s="1">
-        <v>43979</v>
-      </c>
-      <c r="E81" t="s">
-        <v>354</v>
-      </c>
-      <c r="F81" t="s">
-        <v>16</v>
-      </c>
-      <c r="G81" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>356</v>
-      </c>
-      <c r="B82" t="s">
-        <v>357</v>
-      </c>
-      <c r="C82" s="1">
-        <v>43980</v>
-      </c>
-      <c r="D82" s="1">
-        <v>43983</v>
-      </c>
-      <c r="E82" t="s">
-        <v>358</v>
-      </c>
-      <c r="F82" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>360</v>
-      </c>
-      <c r="B83" t="s">
-        <v>361</v>
-      </c>
-      <c r="C83" s="1">
-        <v>43984</v>
-      </c>
-      <c r="D83" s="1">
-        <v>43986</v>
-      </c>
-      <c r="E83" t="s">
-        <v>362</v>
-      </c>
-      <c r="F83" t="s">
-        <v>16</v>
-      </c>
-      <c r="G83" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>364</v>
-      </c>
-      <c r="B84" t="s">
-        <v>365</v>
-      </c>
-      <c r="C84" s="1">
-        <v>43986</v>
-      </c>
-      <c r="D84" s="1">
-        <v>43987</v>
-      </c>
-      <c r="E84" t="s">
-        <v>366</v>
-      </c>
-      <c r="F84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G84" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>367</v>
-      </c>
-      <c r="B85" t="s">
-        <v>368</v>
-      </c>
-      <c r="C85" s="1">
-        <v>43988</v>
-      </c>
-      <c r="D85" s="1">
+      <c r="G85" t="s">
+        <v>374</v>
+      </c>
+      <c r="H85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>375</v>
+      </c>
+      <c r="B86" t="s">
+        <v>376</v>
+      </c>
+      <c r="C86" s="1">
         <v>43990</v>
       </c>
-      <c r="E85" t="s">
-        <v>369</v>
-      </c>
-      <c r="F85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G85" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>371</v>
-      </c>
-      <c r="B86" t="s">
-        <v>372</v>
-      </c>
-      <c r="C86" s="1">
-        <v>43979</v>
-      </c>
       <c r="D86" s="1">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="E86" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="F86" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" t="s">
+        <v>378</v>
+      </c>
+      <c r="H86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>379</v>
+      </c>
+      <c r="B87" t="s">
+        <v>380</v>
+      </c>
+      <c r="C87" s="1">
+        <v>43992</v>
+      </c>
+      <c r="D87" s="1">
+        <v>43994</v>
+      </c>
+      <c r="E87" t="s">
+        <v>381</v>
+      </c>
+      <c r="F87" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" t="s">
+        <v>382</v>
+      </c>
+      <c r="H87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>383</v>
+      </c>
+      <c r="B88" t="s">
+        <v>384</v>
+      </c>
+      <c r="C88" t="s">
+        <v>385</v>
+      </c>
+      <c r="D88" s="1">
+        <v>43996</v>
+      </c>
+      <c r="E88" t="s">
+        <v>386</v>
+      </c>
+      <c r="F88" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" t="s">
+        <v>387</v>
+      </c>
+      <c r="H88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>388</v>
+      </c>
+      <c r="B89" t="s">
+        <v>389</v>
+      </c>
+      <c r="C89" s="1">
+        <v>43997</v>
+      </c>
+      <c r="D89" s="1">
+        <v>43998</v>
+      </c>
+      <c r="E89" t="s">
+        <v>390</v>
+      </c>
+      <c r="F89" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" t="s">
+        <v>391</v>
+      </c>
+      <c r="H89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>392</v>
+      </c>
+      <c r="B90" t="s">
+        <v>393</v>
+      </c>
+      <c r="C90" s="1">
+        <v>43998</v>
+      </c>
+      <c r="D90" s="1">
+        <v>44000</v>
+      </c>
+      <c r="E90" t="s">
+        <v>394</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" t="s">
+        <v>395</v>
+      </c>
+      <c r="H90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>404</v>
+      </c>
+      <c r="B91" t="s">
+        <v>405</v>
+      </c>
+      <c r="C91" s="1">
+        <v>44000</v>
+      </c>
+      <c r="D91" s="1">
+        <v>44002</v>
+      </c>
+      <c r="E91" t="s">
+        <v>406</v>
+      </c>
+      <c r="F91" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" t="s">
+        <v>407</v>
+      </c>
+      <c r="H91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>396</v>
+      </c>
+      <c r="B92" t="s">
+        <v>397</v>
+      </c>
+      <c r="C92" s="1">
+        <v>44002</v>
+      </c>
+      <c r="D92" s="1">
+        <v>44003</v>
+      </c>
+      <c r="E92" t="s">
+        <v>398</v>
+      </c>
+      <c r="F92" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" t="s">
+        <v>399</v>
+      </c>
+      <c r="H92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>400</v>
+      </c>
+      <c r="B93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C93" s="1">
+        <v>44003</v>
+      </c>
+      <c r="D93" s="1">
+        <v>44004</v>
+      </c>
+      <c r="E93" t="s">
+        <v>402</v>
+      </c>
+      <c r="F93" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" t="s">
+        <v>403</v>
+      </c>
+      <c r="H93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>408</v>
+      </c>
+      <c r="B94" t="s">
+        <v>409</v>
+      </c>
+      <c r="C94" s="1">
+        <v>44005</v>
+      </c>
+      <c r="D94" s="1">
+        <v>44011</v>
+      </c>
+      <c r="E94" t="s">
+        <v>410</v>
+      </c>
+      <c r="F94" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" t="s">
+        <v>191</v>
+      </c>
+      <c r="H94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>411</v>
+      </c>
+      <c r="B95" t="s">
+        <v>412</v>
+      </c>
+      <c r="C95" s="1">
+        <v>44007</v>
+      </c>
+      <c r="D95" s="1">
+        <v>44008</v>
+      </c>
+      <c r="E95" t="s">
+        <v>413</v>
+      </c>
+      <c r="F95" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" t="s">
+        <v>414</v>
+      </c>
+      <c r="H95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>415</v>
+      </c>
+      <c r="B96" t="s">
+        <v>416</v>
+      </c>
+      <c r="C96" s="1">
+        <v>44011</v>
+      </c>
+      <c r="D96" s="1">
+        <v>44012</v>
+      </c>
+      <c r="E96" t="s">
+        <v>417</v>
+      </c>
+      <c r="F96" t="s">
         <v>17</v>
       </c>
-      <c r="G86" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>375</v>
-      </c>
-      <c r="B87" t="s">
-        <v>376</v>
-      </c>
-      <c r="C87" s="1">
-        <v>43990</v>
-      </c>
-      <c r="D87" s="1">
-        <v>43992</v>
-      </c>
-      <c r="E87" t="s">
-        <v>377</v>
-      </c>
-      <c r="F87" t="s">
-        <v>16</v>
-      </c>
-      <c r="G87" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>379</v>
-      </c>
-      <c r="B88" t="s">
-        <v>380</v>
-      </c>
-      <c r="C88" s="1">
-        <v>43992</v>
-      </c>
-      <c r="D88" s="1">
-        <v>43994</v>
-      </c>
-      <c r="E88" t="s">
-        <v>381</v>
-      </c>
-      <c r="F88" t="s">
-        <v>16</v>
-      </c>
-      <c r="G88" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>383</v>
-      </c>
-      <c r="B89" t="s">
-        <v>384</v>
-      </c>
-      <c r="C89" t="s">
-        <v>385</v>
-      </c>
-      <c r="D89" s="1">
-        <v>43996</v>
-      </c>
-      <c r="E89" t="s">
-        <v>386</v>
-      </c>
-      <c r="F89" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>388</v>
-      </c>
-      <c r="B90" t="s">
-        <v>389</v>
-      </c>
-      <c r="C90" s="1">
-        <v>43997</v>
-      </c>
-      <c r="D90" s="1">
-        <v>43998</v>
-      </c>
-      <c r="E90" t="s">
-        <v>390</v>
-      </c>
-      <c r="F90" t="s">
-        <v>16</v>
-      </c>
-      <c r="G90" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>392</v>
-      </c>
-      <c r="B91" t="s">
-        <v>393</v>
-      </c>
-      <c r="C91" s="1">
-        <v>43998</v>
-      </c>
-      <c r="D91" s="1">
-        <v>44000</v>
-      </c>
-      <c r="E91" t="s">
-        <v>394</v>
-      </c>
-      <c r="F91" t="s">
-        <v>16</v>
-      </c>
-      <c r="G91" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>404</v>
-      </c>
-      <c r="B92" t="s">
-        <v>405</v>
-      </c>
-      <c r="C92" s="1">
-        <v>44000</v>
-      </c>
-      <c r="D92" s="1">
-        <v>44002</v>
-      </c>
-      <c r="E92" t="s">
-        <v>406</v>
-      </c>
-      <c r="F92" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>396</v>
-      </c>
-      <c r="B93" t="s">
-        <v>397</v>
-      </c>
-      <c r="C93" s="1">
-        <v>44002</v>
-      </c>
-      <c r="D93" s="1">
-        <v>44003</v>
-      </c>
-      <c r="E93" t="s">
-        <v>398</v>
-      </c>
-      <c r="F93" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>400</v>
-      </c>
-      <c r="B94" t="s">
-        <v>401</v>
-      </c>
-      <c r="C94" s="1">
-        <v>44003</v>
-      </c>
-      <c r="D94" s="1">
-        <v>44004</v>
-      </c>
-      <c r="E94" t="s">
-        <v>402</v>
-      </c>
-      <c r="F94" t="s">
-        <v>16</v>
-      </c>
-      <c r="G94" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>408</v>
-      </c>
-      <c r="B95" t="s">
-        <v>409</v>
-      </c>
-      <c r="C95" s="1">
-        <v>44005</v>
-      </c>
-      <c r="D95" s="1">
-        <v>44011</v>
-      </c>
-      <c r="E95" t="s">
-        <v>410</v>
-      </c>
-      <c r="F95" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>411</v>
-      </c>
-      <c r="B96" t="s">
-        <v>412</v>
-      </c>
-      <c r="C96" s="1">
-        <v>44007</v>
-      </c>
-      <c r="D96" s="1">
-        <v>44008</v>
-      </c>
-      <c r="E96" t="s">
-        <v>413</v>
-      </c>
-      <c r="F96" t="s">
-        <v>16</v>
-      </c>
       <c r="G96" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+      <c r="H96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B97" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C97" s="1">
         <v>44011</v>
       </c>
       <c r="D97" s="1">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="E97" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="F97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G97" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+      <c r="H97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B98" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C98" s="1">
-        <v>44011</v>
+        <v>44013</v>
       </c>
       <c r="D98" s="1">
         <v>44013</v>
       </c>
       <c r="E98" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G98" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+      <c r="H98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B99" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="C99" s="1">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D99" s="1">
-        <v>44013</v>
+        <v>44016</v>
       </c>
       <c r="E99" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G99" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+        <v>429</v>
+      </c>
+      <c r="H99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B100" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C100" s="1">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D100" s="1">
         <v>44016</v>
       </c>
       <c r="E100" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
       </c>
       <c r="G100" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+      <c r="H100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B101" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="C101" s="1">
-        <v>44016</v>
+        <v>44014</v>
       </c>
       <c r="D101" s="1">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="E101" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F101" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G101" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+        <v>436</v>
+      </c>
+      <c r="H101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B102" t="s">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="C102" s="1">
-        <v>44014</v>
+        <v>44017</v>
       </c>
       <c r="D102" s="1">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="E102" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="F102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G102" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+      <c r="H102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B103" t="s">
         <v>438</v>
       </c>
       <c r="C103" s="1">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="D103" s="1">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="E103" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="F103" t="s">
         <v>16</v>
       </c>
       <c r="G103" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+      <c r="H103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B104" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C104" s="1">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="D104" s="1">
         <v>44019</v>
       </c>
       <c r="E104" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
       </c>
       <c r="G104" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>444</v>
-      </c>
-      <c r="B105" t="s">
-        <v>445</v>
-      </c>
-      <c r="C105" s="1">
-        <v>44019</v>
-      </c>
-      <c r="D105" s="1">
-        <v>44019</v>
-      </c>
-      <c r="E105" t="s">
-        <v>446</v>
-      </c>
-      <c r="F105" t="s">
-        <v>16</v>
-      </c>
-      <c r="G105" t="s">
         <v>447</v>
+      </c>
+      <c r="H104">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4208,7 +4494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAA95A0-2BF8-4D09-B694-9BB2A3EA2E80}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added whether Ive read the book in the past or not
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3BFE42-F035-4E6F-9871-7F8AAAE93C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A7F491-D6B2-4D4F-A086-445E422C60CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="459">
   <si>
     <t>Title</t>
   </si>
@@ -1409,6 +1409,9 @@
   </si>
   <si>
     <t>Would not recommend</t>
+  </si>
+  <si>
+    <t>First Time Reading?</t>
   </si>
 </sst>
 </file>
@@ -1764,10 +1767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1779,9 +1782,10 @@
     <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1806,8 +1810,11 @@
       <c r="H1" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1832,8 +1839,11 @@
       <c r="H2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1858,8 +1868,11 @@
       <c r="H3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1884,8 +1897,11 @@
       <c r="H4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1910,8 +1926,11 @@
       <c r="H5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1936,8 +1955,11 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1962,8 +1984,11 @@
       <c r="H7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1988,8 +2013,11 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2014,8 +2042,11 @@
       <c r="H9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2040,8 +2071,11 @@
       <c r="H10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2066,8 +2100,11 @@
       <c r="H11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2092,8 +2129,11 @@
       <c r="H12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -2118,8 +2158,11 @@
       <c r="H13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2144,8 +2187,11 @@
       <c r="H14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -2170,8 +2216,11 @@
       <c r="H15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -2196,8 +2245,11 @@
       <c r="H16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -2222,8 +2274,11 @@
       <c r="H17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2248,8 +2303,11 @@
       <c r="H18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2274,8 +2332,11 @@
       <c r="H19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2300,8 +2361,11 @@
       <c r="H20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2326,8 +2390,11 @@
       <c r="H21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2352,8 +2419,11 @@
       <c r="H22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -2378,8 +2448,11 @@
       <c r="H23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -2404,8 +2477,11 @@
       <c r="H24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -2430,8 +2506,11 @@
       <c r="H25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -2456,8 +2535,11 @@
       <c r="H26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -2482,8 +2564,11 @@
       <c r="H27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -2508,8 +2593,11 @@
       <c r="H28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -2534,8 +2622,11 @@
       <c r="H29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -2560,8 +2651,11 @@
       <c r="H30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>165</v>
       </c>
@@ -2586,8 +2680,11 @@
       <c r="H31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>168</v>
       </c>
@@ -2612,8 +2709,11 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -2638,8 +2738,11 @@
       <c r="H33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -2664,8 +2767,11 @@
       <c r="H34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -2690,8 +2796,11 @@
       <c r="H35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -2716,8 +2825,11 @@
       <c r="H36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>189</v>
       </c>
@@ -2742,8 +2854,11 @@
       <c r="H37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -2768,8 +2883,11 @@
       <c r="H38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -2794,8 +2912,11 @@
       <c r="H39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>200</v>
       </c>
@@ -2820,8 +2941,11 @@
       <c r="H40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -2846,8 +2970,11 @@
       <c r="H41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>207</v>
       </c>
@@ -2872,8 +2999,11 @@
       <c r="H42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -2898,8 +3028,11 @@
       <c r="H43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>213</v>
       </c>
@@ -2924,8 +3057,11 @@
       <c r="H44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -2950,8 +3086,11 @@
       <c r="H45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>220</v>
       </c>
@@ -2976,8 +3115,11 @@
       <c r="H46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -3002,8 +3144,11 @@
       <c r="H47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>229</v>
       </c>
@@ -3028,8 +3173,11 @@
       <c r="H48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>233</v>
       </c>
@@ -3054,8 +3202,11 @@
       <c r="H49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -3080,8 +3231,11 @@
       <c r="H50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>240</v>
       </c>
@@ -3106,8 +3260,11 @@
       <c r="H51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>244</v>
       </c>
@@ -3132,8 +3289,11 @@
       <c r="H52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>248</v>
       </c>
@@ -3158,8 +3318,11 @@
       <c r="H53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -3184,8 +3347,11 @@
       <c r="H54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>256</v>
       </c>
@@ -3210,8 +3376,11 @@
       <c r="H55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>260</v>
       </c>
@@ -3236,8 +3405,11 @@
       <c r="H56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>263</v>
       </c>
@@ -3262,8 +3434,11 @@
       <c r="H57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>267</v>
       </c>
@@ -3288,8 +3463,11 @@
       <c r="H58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>271</v>
       </c>
@@ -3314,8 +3492,11 @@
       <c r="H59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -3340,8 +3521,11 @@
       <c r="H60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -3366,8 +3550,11 @@
       <c r="H61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -3392,8 +3579,11 @@
       <c r="H62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>286</v>
       </c>
@@ -3418,8 +3608,11 @@
       <c r="H63">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>290</v>
       </c>
@@ -3444,8 +3637,11 @@
       <c r="H64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>294</v>
       </c>
@@ -3470,8 +3666,11 @@
       <c r="H65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>298</v>
       </c>
@@ -3496,8 +3695,11 @@
       <c r="H66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>302</v>
       </c>
@@ -3522,8 +3724,11 @@
       <c r="H67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>306</v>
       </c>
@@ -3548,8 +3753,11 @@
       <c r="H68">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>310</v>
       </c>
@@ -3574,8 +3782,11 @@
       <c r="H69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>314</v>
       </c>
@@ -3600,8 +3811,11 @@
       <c r="H70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>318</v>
       </c>
@@ -3626,8 +3840,11 @@
       <c r="H71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>322</v>
       </c>
@@ -3652,8 +3869,11 @@
       <c r="H72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>326</v>
       </c>
@@ -3678,8 +3898,11 @@
       <c r="H73">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>330</v>
       </c>
@@ -3704,8 +3927,11 @@
       <c r="H74">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -3730,8 +3956,11 @@
       <c r="H75">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>336</v>
       </c>
@@ -3756,8 +3985,11 @@
       <c r="H76">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>340</v>
       </c>
@@ -3782,8 +4014,11 @@
       <c r="H77">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>344</v>
       </c>
@@ -3808,8 +4043,11 @@
       <c r="H78">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>348</v>
       </c>
@@ -3834,8 +4072,11 @@
       <c r="H79">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>352</v>
       </c>
@@ -3860,8 +4101,11 @@
       <c r="H80">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>356</v>
       </c>
@@ -3886,8 +4130,11 @@
       <c r="H81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>360</v>
       </c>
@@ -3912,8 +4159,11 @@
       <c r="H82">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>364</v>
       </c>
@@ -3938,8 +4188,11 @@
       <c r="H83">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>367</v>
       </c>
@@ -3964,8 +4217,11 @@
       <c r="H84">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>371</v>
       </c>
@@ -3990,8 +4246,11 @@
       <c r="H85">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>375</v>
       </c>
@@ -4016,8 +4275,11 @@
       <c r="H86">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -4042,8 +4304,11 @@
       <c r="H87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>383</v>
       </c>
@@ -4068,8 +4333,11 @@
       <c r="H88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -4094,8 +4362,11 @@
       <c r="H89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>392</v>
       </c>
@@ -4120,8 +4391,11 @@
       <c r="H90">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>404</v>
       </c>
@@ -4146,8 +4420,11 @@
       <c r="H91">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>396</v>
       </c>
@@ -4172,8 +4449,11 @@
       <c r="H92">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>400</v>
       </c>
@@ -4198,8 +4478,11 @@
       <c r="H93">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>408</v>
       </c>
@@ -4224,8 +4507,11 @@
       <c r="H94">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>411</v>
       </c>
@@ -4250,8 +4536,11 @@
       <c r="H95">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>415</v>
       </c>
@@ -4276,8 +4565,11 @@
       <c r="H96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>419</v>
       </c>
@@ -4302,8 +4594,11 @@
       <c r="H97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>423</v>
       </c>
@@ -4328,8 +4623,11 @@
       <c r="H98">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>426</v>
       </c>
@@ -4354,8 +4652,11 @@
       <c r="H99">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>430</v>
       </c>
@@ -4380,8 +4681,11 @@
       <c r="H100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>434</v>
       </c>
@@ -4406,8 +4710,11 @@
       <c r="H101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>437</v>
       </c>
@@ -4432,8 +4739,11 @@
       <c r="H102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>441</v>
       </c>
@@ -4458,8 +4768,11 @@
       <c r="H103">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>444</v>
       </c>
@@ -4483,6 +4796,9 @@
       </c>
       <c r="H104">
         <v>3</v>
+      </c>
+      <c r="I104" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the net and the butterfly and the blind side
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A7F491-D6B2-4D4F-A086-445E422C60CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF9B455-4D29-4E6D-8E77-18825380EC29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="466">
   <si>
     <t>Title</t>
   </si>
@@ -1412,6 +1412,27 @@
   </si>
   <si>
     <t>First Time Reading?</t>
+  </si>
+  <si>
+    <t>The Net and the Bufferfly</t>
+  </si>
+  <si>
+    <t>Olivia Fox Cabane;Judah Pollack</t>
+  </si>
+  <si>
+    <t>eureka;break through;psychology;neuroscience;happiness;productivity;creativity</t>
+  </si>
+  <si>
+    <t>9 Hours 42 Mins</t>
+  </si>
+  <si>
+    <t>The Blind Side</t>
+  </si>
+  <si>
+    <t>football;self improvement;biography;Michael Oherr;redemption</t>
+  </si>
+  <si>
+    <t>11 Hours 49 Mins</t>
   </si>
 </sst>
 </file>
@@ -1767,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I105" sqref="I105"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4798,6 +4819,64 @@
         <v>3</v>
       </c>
       <c r="I104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>459</v>
+      </c>
+      <c r="B105" t="s">
+        <v>460</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44019</v>
+      </c>
+      <c r="D105" s="1">
+        <v>44020</v>
+      </c>
+      <c r="E105" t="s">
+        <v>461</v>
+      </c>
+      <c r="F105" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" t="s">
+        <v>462</v>
+      </c>
+      <c r="H105">
+        <v>3</v>
+      </c>
+      <c r="I105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>463</v>
+      </c>
+      <c r="B106" t="s">
+        <v>438</v>
+      </c>
+      <c r="C106" s="1">
+        <v>44021</v>
+      </c>
+      <c r="D106" s="1">
+        <v>44022</v>
+      </c>
+      <c r="E106" t="s">
+        <v>464</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" t="s">
+        <v>465</v>
+      </c>
+      <c r="H106">
+        <v>4</v>
+      </c>
+      <c r="I106" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the 80/20 principle and the third door
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF9B455-4D29-4E6D-8E77-18825380EC29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4ED7C2-6790-4EFA-BD19-2C67062475B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="474">
   <si>
     <t>Title</t>
   </si>
@@ -1433,6 +1433,30 @@
   </si>
   <si>
     <t>11 Hours 49 Mins</t>
+  </si>
+  <si>
+    <t>The 80/20 Principle and 92 Other Powerful Laws of Nature</t>
+  </si>
+  <si>
+    <t>Richard Koch</t>
+  </si>
+  <si>
+    <t>business;science;success;80/20 rule;darwin;evolution</t>
+  </si>
+  <si>
+    <t>12 Hours 10 Mins</t>
+  </si>
+  <si>
+    <t>The Third Door</t>
+  </si>
+  <si>
+    <t>Alex Banayan</t>
+  </si>
+  <si>
+    <t>success;interviewing;failure;tim ferriss;bill gates;jessica alba;larry king;exponential growth</t>
+  </si>
+  <si>
+    <t>8 Hours 47 Mins</t>
   </si>
 </sst>
 </file>
@@ -1788,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4877,6 +4901,64 @@
         <v>4</v>
       </c>
       <c r="I106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>466</v>
+      </c>
+      <c r="B107" t="s">
+        <v>467</v>
+      </c>
+      <c r="C107" s="1">
+        <v>44022</v>
+      </c>
+      <c r="D107" s="1">
+        <v>44023</v>
+      </c>
+      <c r="E107" t="s">
+        <v>468</v>
+      </c>
+      <c r="F107" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" t="s">
+        <v>469</v>
+      </c>
+      <c r="H107">
+        <v>3</v>
+      </c>
+      <c r="I107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>470</v>
+      </c>
+      <c r="B108" t="s">
+        <v>471</v>
+      </c>
+      <c r="C108" s="1">
+        <v>44024</v>
+      </c>
+      <c r="D108" s="1">
+        <v>44024</v>
+      </c>
+      <c r="E108" t="s">
+        <v>472</v>
+      </c>
+      <c r="F108" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" t="s">
+        <v>473</v>
+      </c>
+      <c r="H108">
+        <v>3</v>
+      </c>
+      <c r="I108" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added no filter and arguing with zombies
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4ED7C2-6790-4EFA-BD19-2C67062475B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7796F99B-5554-457C-B225-6349E4BFEDB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="482">
   <si>
     <t>Title</t>
   </si>
@@ -1457,6 +1457,30 @@
   </si>
   <si>
     <t>8 Hours 47 Mins</t>
+  </si>
+  <si>
+    <t>No Filter</t>
+  </si>
+  <si>
+    <t>Sarah Frier</t>
+  </si>
+  <si>
+    <t>instagram;start-up;facebook;sillicon valley;technology</t>
+  </si>
+  <si>
+    <t>11 Hours 28 Mins</t>
+  </si>
+  <si>
+    <t>Arguing with Zombies</t>
+  </si>
+  <si>
+    <t>Paul Krugman</t>
+  </si>
+  <si>
+    <t>economics;politics;paul krugman;government spending;healthcare</t>
+  </si>
+  <si>
+    <t>12 Hours 22 Mins</t>
   </si>
 </sst>
 </file>
@@ -1812,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4959,6 +4983,64 @@
         <v>3</v>
       </c>
       <c r="I108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>474</v>
+      </c>
+      <c r="B109" t="s">
+        <v>475</v>
+      </c>
+      <c r="C109" s="1">
+        <v>44025</v>
+      </c>
+      <c r="D109" s="1">
+        <v>44026</v>
+      </c>
+      <c r="E109" t="s">
+        <v>476</v>
+      </c>
+      <c r="F109" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" t="s">
+        <v>477</v>
+      </c>
+      <c r="H109">
+        <v>4</v>
+      </c>
+      <c r="I109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>478</v>
+      </c>
+      <c r="B110" t="s">
+        <v>479</v>
+      </c>
+      <c r="C110" s="1">
+        <v>44026</v>
+      </c>
+      <c r="D110" s="1">
+        <v>44028</v>
+      </c>
+      <c r="E110" t="s">
+        <v>480</v>
+      </c>
+      <c r="F110" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" t="s">
+        <v>481</v>
+      </c>
+      <c r="H110">
+        <v>2</v>
+      </c>
+      <c r="I110" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the emperor of all maladies, struck by genius and the medicis
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A1A605-1304-4FD6-9612-44DEF17218D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6C61FB-4A2B-40B7-82A9-BBB58C5792F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="498">
   <si>
     <t>Title</t>
   </si>
@@ -1493,6 +1493,42 @@
   </si>
   <si>
     <t>2 Hours 2 Mins</t>
+  </si>
+  <si>
+    <t>The Emperor of All Maladies</t>
+  </si>
+  <si>
+    <t>Siddrartha Mukherjee</t>
+  </si>
+  <si>
+    <t>cancer;medicine;history;science;disease</t>
+  </si>
+  <si>
+    <t>20 Hours 46 Mins</t>
+  </si>
+  <si>
+    <t>Struck by Genius</t>
+  </si>
+  <si>
+    <t>Jason Padgett</t>
+  </si>
+  <si>
+    <t>math;autobiography;genius;savant</t>
+  </si>
+  <si>
+    <t>268 Pages</t>
+  </si>
+  <si>
+    <t>The Medici</t>
+  </si>
+  <si>
+    <t>Paul Stratham</t>
+  </si>
+  <si>
+    <t>italy;medici;history;renaisance;europe</t>
+  </si>
+  <si>
+    <t>16 Hours 22 Mins</t>
   </si>
 </sst>
 </file>
@@ -1848,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5082,6 +5118,93 @@
         <v>3</v>
       </c>
       <c r="I111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>486</v>
+      </c>
+      <c r="B112" t="s">
+        <v>487</v>
+      </c>
+      <c r="C112" s="1">
+        <v>44031</v>
+      </c>
+      <c r="D112" s="1">
+        <v>44037</v>
+      </c>
+      <c r="E112" t="s">
+        <v>488</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" t="s">
+        <v>489</v>
+      </c>
+      <c r="H112">
+        <v>3</v>
+      </c>
+      <c r="I112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>490</v>
+      </c>
+      <c r="B113" t="s">
+        <v>491</v>
+      </c>
+      <c r="C113" s="1">
+        <v>44018</v>
+      </c>
+      <c r="D113" s="1">
+        <v>44033</v>
+      </c>
+      <c r="E113" t="s">
+        <v>492</v>
+      </c>
+      <c r="F113" t="s">
+        <v>141</v>
+      </c>
+      <c r="G113" t="s">
+        <v>493</v>
+      </c>
+      <c r="H113">
+        <v>2</v>
+      </c>
+      <c r="I113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>494</v>
+      </c>
+      <c r="B114" t="s">
+        <v>495</v>
+      </c>
+      <c r="C114" s="1">
+        <v>44038</v>
+      </c>
+      <c r="D114" s="1">
+        <v>44041</v>
+      </c>
+      <c r="E114" t="s">
+        <v>496</v>
+      </c>
+      <c r="F114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>497</v>
+      </c>
+      <c r="H114">
+        <v>3</v>
+      </c>
+      <c r="I114" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added salt, guns germs and steel, get well soon
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6C61FB-4A2B-40B7-82A9-BBB58C5792F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C67DCD3-28C3-4E23-812A-DD0EDD70C971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="510">
   <si>
     <t>Title</t>
   </si>
@@ -1529,6 +1529,42 @@
   </si>
   <si>
     <t>16 Hours 22 Mins</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Mark Kurlansky</t>
+  </si>
+  <si>
+    <t>history;salt;cuisine;food;fish</t>
+  </si>
+  <si>
+    <t>Guns, Germs and Steel</t>
+  </si>
+  <si>
+    <t>Jared Diamond</t>
+  </si>
+  <si>
+    <t>history;society;slavery;conquest;western culture;hunters &amp; gatherers;farming;disease</t>
+  </si>
+  <si>
+    <t>Get Well Soon</t>
+  </si>
+  <si>
+    <t>Jennifer Wright</t>
+  </si>
+  <si>
+    <t>history;disease;spanish flu;pandemic;aids;cholera;polio;lobotomy;bubonic plague;dancing plague;smallpox;syphilis;tuberculosis;leprosy;encephalitis lethargica;medicine;vaccine</t>
+  </si>
+  <si>
+    <t>16 Hours 21 Mins</t>
+  </si>
+  <si>
+    <t>7 Hours 49 Mins</t>
+  </si>
+  <si>
+    <t>13 Hours 49 Mins</t>
   </si>
 </sst>
 </file>
@@ -1884,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5205,6 +5241,93 @@
         <v>3</v>
       </c>
       <c r="I114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>498</v>
+      </c>
+      <c r="B115" t="s">
+        <v>499</v>
+      </c>
+      <c r="C115" s="1">
+        <v>44041</v>
+      </c>
+      <c r="D115" s="1">
+        <v>44045</v>
+      </c>
+      <c r="E115" t="s">
+        <v>500</v>
+      </c>
+      <c r="F115" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" t="s">
+        <v>509</v>
+      </c>
+      <c r="H115">
+        <v>3</v>
+      </c>
+      <c r="I115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>501</v>
+      </c>
+      <c r="B116" t="s">
+        <v>502</v>
+      </c>
+      <c r="C116" s="1">
+        <v>44045</v>
+      </c>
+      <c r="D116" s="1">
+        <v>44048</v>
+      </c>
+      <c r="E116" t="s">
+        <v>503</v>
+      </c>
+      <c r="F116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" t="s">
+        <v>507</v>
+      </c>
+      <c r="H116">
+        <v>3</v>
+      </c>
+      <c r="I116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>504</v>
+      </c>
+      <c r="B117" t="s">
+        <v>505</v>
+      </c>
+      <c r="C117" s="1">
+        <v>44048</v>
+      </c>
+      <c r="D117" s="1">
+        <v>44049</v>
+      </c>
+      <c r="E117" t="s">
+        <v>506</v>
+      </c>
+      <c r="F117" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" t="s">
+        <v>508</v>
+      </c>
+      <c r="H117">
+        <v>4</v>
+      </c>
+      <c r="I117" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added american moonshot and lords of finance
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E574FC-4F5D-416E-8678-8A73D934D633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CBF336-0274-4B94-9506-0FC167492BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="522">
   <si>
     <t>Title</t>
   </si>
@@ -1577,6 +1577,30 @@
   </si>
   <si>
     <t>16 Hours 39 Mins</t>
+  </si>
+  <si>
+    <t>American Moonshot</t>
+  </si>
+  <si>
+    <t>Douglas Brinkley</t>
+  </si>
+  <si>
+    <t>space race;cold war;history;john f kennedy;moon landing</t>
+  </si>
+  <si>
+    <t>17 Hours 23 Mins</t>
+  </si>
+  <si>
+    <t>Lords of Finance</t>
+  </si>
+  <si>
+    <t>Liaquat Ahamed</t>
+  </si>
+  <si>
+    <t>history;world war 1;world war 2;finance;reparations;great depression</t>
+  </si>
+  <si>
+    <t>505 Pages</t>
   </si>
 </sst>
 </file>
@@ -1932,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5369,6 +5393,64 @@
         <v>3</v>
       </c>
       <c r="I118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>514</v>
+      </c>
+      <c r="B119" t="s">
+        <v>515</v>
+      </c>
+      <c r="C119" s="1">
+        <v>44053</v>
+      </c>
+      <c r="D119" s="1">
+        <v>44056</v>
+      </c>
+      <c r="E119" t="s">
+        <v>516</v>
+      </c>
+      <c r="F119" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" t="s">
+        <v>517</v>
+      </c>
+      <c r="H119">
+        <v>3</v>
+      </c>
+      <c r="I119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>518</v>
+      </c>
+      <c r="B120" t="s">
+        <v>519</v>
+      </c>
+      <c r="C120" s="1">
+        <v>44034</v>
+      </c>
+      <c r="D120" s="1">
+        <v>44057</v>
+      </c>
+      <c r="E120" t="s">
+        <v>520</v>
+      </c>
+      <c r="F120" t="s">
+        <v>17</v>
+      </c>
+      <c r="G120" t="s">
+        <v>521</v>
+      </c>
+      <c r="H120">
+        <v>3</v>
+      </c>
+      <c r="I120" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the deviants war
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CBF336-0274-4B94-9506-0FC167492BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698730CC-E2EE-49E5-B1B4-094D40D59F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="526">
   <si>
     <t>Title</t>
   </si>
@@ -1601,6 +1601,18 @@
   </si>
   <si>
     <t>505 Pages</t>
+  </si>
+  <si>
+    <t>The Deviants War</t>
+  </si>
+  <si>
+    <t>Eric Cervini</t>
+  </si>
+  <si>
+    <t>history;gay rights;legal battles;jay edgar hoover;government;persecution</t>
+  </si>
+  <si>
+    <t>15 Hours 43 Mins</t>
   </si>
 </sst>
 </file>
@@ -1956,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5451,6 +5463,35 @@
         <v>3</v>
       </c>
       <c r="I120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>522</v>
+      </c>
+      <c r="B121" t="s">
+        <v>523</v>
+      </c>
+      <c r="C121" s="1">
+        <v>44057</v>
+      </c>
+      <c r="D121" s="1">
+        <v>44060</v>
+      </c>
+      <c r="E121" t="s">
+        <v>524</v>
+      </c>
+      <c r="F121" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" t="s">
+        <v>525</v>
+      </c>
+      <c r="H121">
+        <v>3</v>
+      </c>
+      <c r="I121" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a bookshop in berlin
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9572ED8-9221-4F37-AC63-591D5A4A16C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B9E8B3-0EB1-4DD5-9EC7-AA18A14C9470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="533">
   <si>
     <t>Title</t>
   </si>
@@ -1622,6 +1622,18 @@
   </si>
   <si>
     <t>7 Hours 43 Mins</t>
+  </si>
+  <si>
+    <t>A Bookshop in Berlin</t>
+  </si>
+  <si>
+    <t>Francoise Frenkel</t>
+  </si>
+  <si>
+    <t>memoir;nazi;world war 2;holocaust;judaism;survival</t>
+  </si>
+  <si>
+    <t>6 Hours 30 Mins</t>
   </si>
 </sst>
 </file>
@@ -1977,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5530,6 +5542,35 @@
         <v>3</v>
       </c>
       <c r="I122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>529</v>
+      </c>
+      <c r="B123" t="s">
+        <v>530</v>
+      </c>
+      <c r="C123" s="1">
+        <v>44063</v>
+      </c>
+      <c r="D123" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E123" t="s">
+        <v>531</v>
+      </c>
+      <c r="F123" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" t="s">
+        <v>532</v>
+      </c>
+      <c r="H123">
+        <v>4</v>
+      </c>
+      <c r="I123" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the new tsar
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B9E8B3-0EB1-4DD5-9EC7-AA18A14C9470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF3B908-9724-4EB6-B79B-5E6052243AC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7360" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="537">
   <si>
     <t>Title</t>
   </si>
@@ -1634,6 +1634,18 @@
   </si>
   <si>
     <t>6 Hours 30 Mins</t>
+  </si>
+  <si>
+    <t>The New Tsar</t>
+  </si>
+  <si>
+    <t>Steven Lee Myers</t>
+  </si>
+  <si>
+    <t>biography;politics;russia;vladimir putin;history</t>
+  </si>
+  <si>
+    <t>22 Hours 55 Mins</t>
   </si>
 </sst>
 </file>
@@ -1989,10 +2001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5572,6 +5584,32 @@
       </c>
       <c r="I123" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>533</v>
+      </c>
+      <c r="B124" t="s">
+        <v>534</v>
+      </c>
+      <c r="C124" s="1">
+        <v>44064</v>
+      </c>
+      <c r="D124" s="1">
+        <v>44071</v>
+      </c>
+      <c r="E124" t="s">
+        <v>535</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" t="s">
+        <v>536</v>
+      </c>
+      <c r="H124">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the guns of august
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF3B908-9724-4EB6-B79B-5E6052243AC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DAC06F-EBEC-47AF-B4A2-DA511D8E4538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7360" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="541">
   <si>
     <t>Title</t>
   </si>
@@ -1646,6 +1646,18 @@
   </si>
   <si>
     <t>22 Hours 55 Mins</t>
+  </si>
+  <si>
+    <t>The Guns of August</t>
+  </si>
+  <si>
+    <t>Barbara Tuchman</t>
+  </si>
+  <si>
+    <t>history;world war 1;war;europe</t>
+  </si>
+  <si>
+    <t>19 Hours 18 Mins</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="D112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K126" sqref="K126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5610,6 +5622,38 @@
       </c>
       <c r="H124">
         <v>3</v>
+      </c>
+      <c r="I124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>537</v>
+      </c>
+      <c r="B125" t="s">
+        <v>538</v>
+      </c>
+      <c r="C125" s="1">
+        <v>44072</v>
+      </c>
+      <c r="D125" s="1">
+        <v>44078</v>
+      </c>
+      <c r="E125" t="s">
+        <v>539</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" t="s">
+        <v>540</v>
+      </c>
+      <c r="H125">
+        <v>3</v>
+      </c>
+      <c r="I125" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cleopatra and the african samurai
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DAC06F-EBEC-47AF-B4A2-DA511D8E4538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B41C5-4426-41B4-954D-44989279ADAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7360" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="549">
   <si>
     <t>Title</t>
   </si>
@@ -1658,6 +1658,30 @@
   </si>
   <si>
     <t>19 Hours 18 Mins</t>
+  </si>
+  <si>
+    <t>Cleopatra</t>
+  </si>
+  <si>
+    <t>Stacy Schiff</t>
+  </si>
+  <si>
+    <t>biography;egypt;rome;history;alexandria;cleopatra;julius caesar;mark antony;alexander the great;war;politics</t>
+  </si>
+  <si>
+    <t>14 Hours 17 Mins</t>
+  </si>
+  <si>
+    <t>African Samurai</t>
+  </si>
+  <si>
+    <t>Thomas Lockley</t>
+  </si>
+  <si>
+    <t>biography;history;japan;samurai;slavery;war</t>
+  </si>
+  <si>
+    <t>10 Hours 13 Mins</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K126" sqref="K126"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5654,6 +5678,58 @@
       </c>
       <c r="I125" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>541</v>
+      </c>
+      <c r="B126" t="s">
+        <v>542</v>
+      </c>
+      <c r="C126" s="1">
+        <v>44078</v>
+      </c>
+      <c r="D126" s="1">
+        <v>44080</v>
+      </c>
+      <c r="E126" t="s">
+        <v>543</v>
+      </c>
+      <c r="F126" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" t="s">
+        <v>544</v>
+      </c>
+      <c r="H126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>545</v>
+      </c>
+      <c r="B127" t="s">
+        <v>546</v>
+      </c>
+      <c r="C127" s="1">
+        <v>44080</v>
+      </c>
+      <c r="D127" s="1">
+        <v>44083</v>
+      </c>
+      <c r="E127" t="s">
+        <v>547</v>
+      </c>
+      <c r="F127" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127" t="s">
+        <v>548</v>
+      </c>
+      <c r="H127">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added road to jonestown and the boys in the boat
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B41C5-4426-41B4-954D-44989279ADAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAAA8C3-76A8-4392-8252-72CDF5DD2100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7360" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="557">
   <si>
     <t>Title</t>
   </si>
@@ -1682,6 +1682,30 @@
   </si>
   <si>
     <t>10 Hours 13 Mins</t>
+  </si>
+  <si>
+    <t>The Boys in the Boat</t>
+  </si>
+  <si>
+    <t>Daniel James Brown</t>
+  </si>
+  <si>
+    <t>history;rowing;olympics;biography;sports;triumph</t>
+  </si>
+  <si>
+    <t>14 Hours 11 Mins</t>
+  </si>
+  <si>
+    <t>17 Hours 30 Mins</t>
+  </si>
+  <si>
+    <t>Road to Jonestown</t>
+  </si>
+  <si>
+    <t>Jeff Guinn</t>
+  </si>
+  <si>
+    <t>biography;history;jonestown;cults;mass suicide</t>
   </si>
 </sst>
 </file>
@@ -2037,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5705,6 +5729,9 @@
       <c r="H126">
         <v>3</v>
       </c>
+      <c r="I126" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
@@ -5730,6 +5757,67 @@
       </c>
       <c r="H127">
         <v>3</v>
+      </c>
+      <c r="I127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>554</v>
+      </c>
+      <c r="B128" t="s">
+        <v>555</v>
+      </c>
+      <c r="C128" s="1">
+        <v>44083</v>
+      </c>
+      <c r="D128" s="1">
+        <v>44086</v>
+      </c>
+      <c r="E128" t="s">
+        <v>556</v>
+      </c>
+      <c r="F128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" t="s">
+        <v>553</v>
+      </c>
+      <c r="H128">
+        <v>3</v>
+      </c>
+      <c r="I128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>549</v>
+      </c>
+      <c r="B129" t="s">
+        <v>550</v>
+      </c>
+      <c r="C129" s="1">
+        <v>44087</v>
+      </c>
+      <c r="D129" s="1">
+        <v>44096</v>
+      </c>
+      <c r="E129" t="s">
+        <v>551</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" t="s">
+        <v>552</v>
+      </c>
+      <c r="H129">
+        <v>3</v>
+      </c>
+      <c r="I129" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added own the day own your life
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617CEE84-FFBE-4D1D-BE0D-FA02A5E152E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD159426-595D-42EC-8A92-5AB1A146CA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="569">
   <si>
     <t>Title</t>
   </si>
@@ -1730,6 +1730,18 @@
   </si>
   <si>
     <t>14 Hours 45 Mins</t>
+  </si>
+  <si>
+    <t>Own the Day, Own Your Life</t>
+  </si>
+  <si>
+    <t>Aubrey Marcus</t>
+  </si>
+  <si>
+    <t>health;optimal health;optimal performance;diet;sleep;exercise</t>
+  </si>
+  <si>
+    <t>11 Hours 5 Mins</t>
   </si>
 </sst>
 </file>
@@ -2085,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5899,6 +5911,35 @@
         <v>3</v>
       </c>
       <c r="I131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>565</v>
+      </c>
+      <c r="B132" t="s">
+        <v>566</v>
+      </c>
+      <c r="C132" s="1">
+        <v>44104</v>
+      </c>
+      <c r="D132" s="1">
+        <v>44106</v>
+      </c>
+      <c r="E132" t="s">
+        <v>567</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" t="s">
+        <v>568</v>
+      </c>
+      <c r="H132">
+        <v>2</v>
+      </c>
+      <c r="I132" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 168 Hours and how to think like a roman emperor
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97958BDA-ED1E-4D23-B39C-BDDA98F7B5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8F1933-5615-4B62-B6BA-F0A3C348F9CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="580">
   <si>
     <t>Title</t>
   </si>
@@ -1754,6 +1754,27 @@
   </si>
   <si>
     <t>9 Hours 44 Mins</t>
+  </si>
+  <si>
+    <t>How to Think Like a Roman Emperor</t>
+  </si>
+  <si>
+    <t>Donald Robertson</t>
+  </si>
+  <si>
+    <t>stoic;marcus aurelius;philosophy;history</t>
+  </si>
+  <si>
+    <t>8 Hours 36 Mins</t>
+  </si>
+  <si>
+    <t>168 Hours</t>
+  </si>
+  <si>
+    <t>productivity;time management;achievement;personal improvement</t>
+  </si>
+  <si>
+    <t>7 Hours 48 Mins</t>
   </si>
 </sst>
 </file>
@@ -2109,10 +2130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5978,6 +5999,67 @@
       </c>
       <c r="H133">
         <v>3</v>
+      </c>
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>573</v>
+      </c>
+      <c r="B134" t="s">
+        <v>574</v>
+      </c>
+      <c r="C134" s="1">
+        <v>44124</v>
+      </c>
+      <c r="D134" s="1">
+        <v>44126</v>
+      </c>
+      <c r="E134" t="s">
+        <v>575</v>
+      </c>
+      <c r="F134" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" t="s">
+        <v>576</v>
+      </c>
+      <c r="H134">
+        <v>3</v>
+      </c>
+      <c r="I134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>577</v>
+      </c>
+      <c r="B135" t="s">
+        <v>445</v>
+      </c>
+      <c r="C135" s="1">
+        <v>44126</v>
+      </c>
+      <c r="D135" s="1">
+        <v>44128</v>
+      </c>
+      <c r="E135" t="s">
+        <v>578</v>
+      </c>
+      <c r="F135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" t="s">
+        <v>579</v>
+      </c>
+      <c r="H135">
+        <v>4</v>
+      </c>
+      <c r="I135" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added george lucas and buffett
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0ED1D1-17B8-4A76-88CC-81BB67842E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA00493-1E71-476C-83FD-B972C4AE433F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="592">
   <si>
     <t>Title</t>
   </si>
@@ -1787,6 +1787,30 @@
   </si>
   <si>
     <t>13 Hours 19 Mins</t>
+  </si>
+  <si>
+    <t>George Lucas: A Life</t>
+  </si>
+  <si>
+    <t>Brian Jay Jones</t>
+  </si>
+  <si>
+    <t>biography;history;george lucas;star wars;hollywood;cinema;indiana jones</t>
+  </si>
+  <si>
+    <t>18 Hours 18 Mins</t>
+  </si>
+  <si>
+    <t>Buffett</t>
+  </si>
+  <si>
+    <t>Roger Lowenstein</t>
+  </si>
+  <si>
+    <t>biography;warren buffett;finance;investing</t>
+  </si>
+  <si>
+    <t>423 Pages</t>
   </si>
 </sst>
 </file>
@@ -2142,24 +2166,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2188,7 +2212,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2217,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2246,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2275,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2333,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2362,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2420,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2449,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2478,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2507,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -2536,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2565,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -2594,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -2652,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2681,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2710,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2739,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2768,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2797,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -2826,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -2855,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -2884,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -2913,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -2942,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -2971,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -3000,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -3029,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>165</v>
       </c>
@@ -3058,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>168</v>
       </c>
@@ -3087,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -3116,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -3145,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -3174,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -3203,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>189</v>
       </c>
@@ -3232,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -3261,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -3290,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>200</v>
       </c>
@@ -3319,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -3348,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>207</v>
       </c>
@@ -3377,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3406,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>213</v>
       </c>
@@ -3435,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -3464,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>220</v>
       </c>
@@ -3493,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -3522,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>229</v>
       </c>
@@ -3551,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>233</v>
       </c>
@@ -3580,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -3609,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>240</v>
       </c>
@@ -3638,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>244</v>
       </c>
@@ -3667,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>248</v>
       </c>
@@ -3696,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -3725,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>256</v>
       </c>
@@ -3754,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>260</v>
       </c>
@@ -3783,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>263</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>267</v>
       </c>
@@ -3841,7 +3865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>271</v>
       </c>
@@ -3870,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -3899,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -3928,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -3957,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>286</v>
       </c>
@@ -3986,7 +4010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>290</v>
       </c>
@@ -4015,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>294</v>
       </c>
@@ -4044,7 +4068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>298</v>
       </c>
@@ -4073,7 +4097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>302</v>
       </c>
@@ -4102,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>306</v>
       </c>
@@ -4131,7 +4155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>310</v>
       </c>
@@ -4160,7 +4184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>314</v>
       </c>
@@ -4189,7 +4213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>318</v>
       </c>
@@ -4218,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>322</v>
       </c>
@@ -4247,7 +4271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>326</v>
       </c>
@@ -4276,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>330</v>
       </c>
@@ -4305,7 +4329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -4334,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>336</v>
       </c>
@@ -4363,7 +4387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>340</v>
       </c>
@@ -4392,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>344</v>
       </c>
@@ -4421,7 +4445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>348</v>
       </c>
@@ -4450,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>352</v>
       </c>
@@ -4479,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>356</v>
       </c>
@@ -4508,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>360</v>
       </c>
@@ -4537,7 +4561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>364</v>
       </c>
@@ -4566,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>367</v>
       </c>
@@ -4595,7 +4619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>371</v>
       </c>
@@ -4624,7 +4648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>375</v>
       </c>
@@ -4653,7 +4677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -4682,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>383</v>
       </c>
@@ -4711,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -4740,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>392</v>
       </c>
@@ -4769,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>404</v>
       </c>
@@ -4798,7 +4822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>396</v>
       </c>
@@ -4827,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>400</v>
       </c>
@@ -4856,7 +4880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>408</v>
       </c>
@@ -4885,7 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>411</v>
       </c>
@@ -4914,7 +4938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>415</v>
       </c>
@@ -4943,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>419</v>
       </c>
@@ -4972,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>423</v>
       </c>
@@ -5001,7 +5025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>426</v>
       </c>
@@ -5030,7 +5054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>430</v>
       </c>
@@ -5059,7 +5083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>434</v>
       </c>
@@ -5088,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>437</v>
       </c>
@@ -5117,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>441</v>
       </c>
@@ -5146,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>444</v>
       </c>
@@ -5175,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>459</v>
       </c>
@@ -5204,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>463</v>
       </c>
@@ -5233,7 +5257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>466</v>
       </c>
@@ -5262,7 +5286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>470</v>
       </c>
@@ -5291,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>474</v>
       </c>
@@ -5320,7 +5344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>478</v>
       </c>
@@ -5349,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>482</v>
       </c>
@@ -5378,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>486</v>
       </c>
@@ -5407,7 +5431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>490</v>
       </c>
@@ -5436,7 +5460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>494</v>
       </c>
@@ -5465,7 +5489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>498</v>
       </c>
@@ -5494,7 +5518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>501</v>
       </c>
@@ -5523,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>504</v>
       </c>
@@ -5552,7 +5576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>510</v>
       </c>
@@ -5581,7 +5605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>514</v>
       </c>
@@ -5610,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>518</v>
       </c>
@@ -5639,7 +5663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>522</v>
       </c>
@@ -5668,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>41</v>
       </c>
@@ -5697,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>529</v>
       </c>
@@ -5726,7 +5750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>533</v>
       </c>
@@ -5755,7 +5779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>537</v>
       </c>
@@ -5784,7 +5808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>541</v>
       </c>
@@ -5813,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>545</v>
       </c>
@@ -5842,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>554</v>
       </c>
@@ -5871,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>549</v>
       </c>
@@ -5900,7 +5924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>557</v>
       </c>
@@ -5929,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>561</v>
       </c>
@@ -5958,7 +5982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>565</v>
       </c>
@@ -5987,7 +6011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>569</v>
       </c>
@@ -6016,7 +6040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>573</v>
       </c>
@@ -6045,7 +6069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>577</v>
       </c>
@@ -6074,7 +6098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>580</v>
       </c>
@@ -6100,6 +6124,64 @@
         <v>4</v>
       </c>
       <c r="I136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>584</v>
+      </c>
+      <c r="B137" t="s">
+        <v>585</v>
+      </c>
+      <c r="C137" s="1">
+        <v>44130</v>
+      </c>
+      <c r="D137" s="1">
+        <v>44132</v>
+      </c>
+      <c r="E137" t="s">
+        <v>586</v>
+      </c>
+      <c r="F137" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" t="s">
+        <v>587</v>
+      </c>
+      <c r="H137">
+        <v>4</v>
+      </c>
+      <c r="I137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>588</v>
+      </c>
+      <c r="B138" t="s">
+        <v>589</v>
+      </c>
+      <c r="C138" s="1">
+        <v>44100</v>
+      </c>
+      <c r="D138" s="1">
+        <v>44133</v>
+      </c>
+      <c r="E138" t="s">
+        <v>590</v>
+      </c>
+      <c r="F138" t="s">
+        <v>17</v>
+      </c>
+      <c r="G138" t="s">
+        <v>591</v>
+      </c>
+      <c r="H138">
+        <v>3</v>
+      </c>
+      <c r="I138" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6116,13 +6198,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -6133,7 +6215,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>452</v>
       </c>
@@ -6144,7 +6226,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>452</v>
       </c>
@@ -6155,7 +6237,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>452</v>
       </c>
@@ -6166,7 +6248,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -6177,7 +6259,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>452</v>
       </c>
@@ -6201,13 +6283,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6215,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -6223,7 +6305,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -6231,7 +6313,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -6239,7 +6321,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -6247,7 +6329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -6255,7 +6337,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -6263,7 +6345,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -6271,7 +6353,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -6279,7 +6361,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -6287,7 +6369,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -6295,7 +6377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -6303,7 +6385,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -6311,7 +6393,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -6319,7 +6401,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -6327,7 +6409,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -6335,7 +6417,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -6343,7 +6425,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -6351,7 +6433,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -6359,7 +6441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -6367,7 +6449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -6375,7 +6457,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added a ride of a lifetime
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA00493-1E71-476C-83FD-B972C4AE433F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080CBDA6-DC91-446F-A3DF-1E042033EE2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="596">
   <si>
     <t>Title</t>
   </si>
@@ -1811,6 +1811,18 @@
   </si>
   <si>
     <t>423 Pages</t>
+  </si>
+  <si>
+    <t>A Ride of a Lifetime</t>
+  </si>
+  <si>
+    <t>Robert Iger</t>
+  </si>
+  <si>
+    <t>biography;memoir;bob iger;disney;abc;success;career</t>
+  </si>
+  <si>
+    <t>8 Hours 45 Mins</t>
   </si>
 </sst>
 </file>
@@ -2166,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+      <selection activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6182,6 +6194,35 @@
         <v>3</v>
       </c>
       <c r="I138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>592</v>
+      </c>
+      <c r="B139" t="s">
+        <v>593</v>
+      </c>
+      <c r="C139" s="1">
+        <v>44133</v>
+      </c>
+      <c r="D139" s="1">
+        <v>44133</v>
+      </c>
+      <c r="E139" t="s">
+        <v>594</v>
+      </c>
+      <c r="F139" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" t="s">
+        <v>595</v>
+      </c>
+      <c r="H139">
+        <v>4</v>
+      </c>
+      <c r="I139" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the compound effect
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2A3513-75B0-4A70-AB8F-0D47C1AF8EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5902AF-B632-41BF-B072-6080C34FB2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="604">
   <si>
     <t>Title</t>
   </si>
@@ -1835,6 +1835,18 @@
   </si>
   <si>
     <t>6 Hours 48 Mins</t>
+  </si>
+  <si>
+    <t>The Compound Effect</t>
+  </si>
+  <si>
+    <t>Darren Hardy</t>
+  </si>
+  <si>
+    <t>personal development;motivation;habits;success</t>
+  </si>
+  <si>
+    <t>4 Hours 44 Mins</t>
   </si>
 </sst>
 </file>
@@ -2190,24 +2202,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2248,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2265,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2323,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2352,7 +2364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2381,7 +2393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2410,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2439,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2468,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2526,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2555,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -2584,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2613,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -2700,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2729,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2758,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2816,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2845,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1491</v>
       </c>
@@ -2874,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -2903,7 +2915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -2932,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -2961,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -2990,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -3019,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -3077,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>165</v>
       </c>
@@ -3106,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>168</v>
       </c>
@@ -3135,7 +3147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -3193,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -3222,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -3251,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>189</v>
       </c>
@@ -3280,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -3309,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -3338,7 +3350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>200</v>
       </c>
@@ -3367,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -3396,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>207</v>
       </c>
@@ -3425,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3454,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>213</v>
       </c>
@@ -3483,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -3512,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>220</v>
       </c>
@@ -3541,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -3570,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>229</v>
       </c>
@@ -3599,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>233</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -3657,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>240</v>
       </c>
@@ -3686,7 +3698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>244</v>
       </c>
@@ -3715,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>248</v>
       </c>
@@ -3744,7 +3756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -3773,7 +3785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>256</v>
       </c>
@@ -3802,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>260</v>
       </c>
@@ -3831,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>263</v>
       </c>
@@ -3860,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>267</v>
       </c>
@@ -3889,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>271</v>
       </c>
@@ -3918,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -3947,7 +3959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -3976,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -4005,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>286</v>
       </c>
@@ -4034,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>290</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>294</v>
       </c>
@@ -4092,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>298</v>
       </c>
@@ -4121,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>302</v>
       </c>
@@ -4150,7 +4162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>306</v>
       </c>
@@ -4179,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>310</v>
       </c>
@@ -4208,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>314</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>318</v>
       </c>
@@ -4266,7 +4278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>322</v>
       </c>
@@ -4295,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>326</v>
       </c>
@@ -4324,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>330</v>
       </c>
@@ -4353,7 +4365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>336</v>
       </c>
@@ -4411,7 +4423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>340</v>
       </c>
@@ -4440,7 +4452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>344</v>
       </c>
@@ -4469,7 +4481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>348</v>
       </c>
@@ -4498,7 +4510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>352</v>
       </c>
@@ -4527,7 +4539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>356</v>
       </c>
@@ -4556,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>360</v>
       </c>
@@ -4585,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>364</v>
       </c>
@@ -4614,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>367</v>
       </c>
@@ -4643,7 +4655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>371</v>
       </c>
@@ -4672,7 +4684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>375</v>
       </c>
@@ -4701,7 +4713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -4730,7 +4742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>383</v>
       </c>
@@ -4759,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -4788,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>392</v>
       </c>
@@ -4817,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>404</v>
       </c>
@@ -4846,7 +4858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>396</v>
       </c>
@@ -4875,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>400</v>
       </c>
@@ -4904,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>408</v>
       </c>
@@ -4933,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>411</v>
       </c>
@@ -4962,7 +4974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>415</v>
       </c>
@@ -4991,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>419</v>
       </c>
@@ -5020,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>423</v>
       </c>
@@ -5049,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>426</v>
       </c>
@@ -5078,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>430</v>
       </c>
@@ -5107,7 +5119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>434</v>
       </c>
@@ -5136,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>437</v>
       </c>
@@ -5165,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>441</v>
       </c>
@@ -5194,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>444</v>
       </c>
@@ -5223,7 +5235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>459</v>
       </c>
@@ -5252,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>463</v>
       </c>
@@ -5281,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>466</v>
       </c>
@@ -5310,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>470</v>
       </c>
@@ -5339,7 +5351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>474</v>
       </c>
@@ -5368,7 +5380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>478</v>
       </c>
@@ -5397,7 +5409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>482</v>
       </c>
@@ -5426,7 +5438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>486</v>
       </c>
@@ -5455,7 +5467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>490</v>
       </c>
@@ -5484,7 +5496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>494</v>
       </c>
@@ -5513,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>498</v>
       </c>
@@ -5542,7 +5554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>501</v>
       </c>
@@ -5571,7 +5583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>504</v>
       </c>
@@ -5600,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>510</v>
       </c>
@@ -5629,7 +5641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>514</v>
       </c>
@@ -5658,7 +5670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>518</v>
       </c>
@@ -5687,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>522</v>
       </c>
@@ -5716,7 +5728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>41</v>
       </c>
@@ -5745,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>529</v>
       </c>
@@ -5774,7 +5786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>533</v>
       </c>
@@ -5803,7 +5815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>537</v>
       </c>
@@ -5832,7 +5844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>541</v>
       </c>
@@ -5861,7 +5873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>545</v>
       </c>
@@ -5890,7 +5902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>554</v>
       </c>
@@ -5919,7 +5931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>549</v>
       </c>
@@ -5948,7 +5960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>557</v>
       </c>
@@ -5977,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>561</v>
       </c>
@@ -6006,7 +6018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>565</v>
       </c>
@@ -6035,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>569</v>
       </c>
@@ -6064,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>573</v>
       </c>
@@ -6093,7 +6105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>577</v>
       </c>
@@ -6122,7 +6134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>580</v>
       </c>
@@ -6151,7 +6163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>584</v>
       </c>
@@ -6180,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>588</v>
       </c>
@@ -6209,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>592</v>
       </c>
@@ -6238,7 +6250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>596</v>
       </c>
@@ -6265,6 +6277,35 @@
       </c>
       <c r="I140" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>600</v>
+      </c>
+      <c r="B141" t="s">
+        <v>601</v>
+      </c>
+      <c r="C141" s="1">
+        <v>44136</v>
+      </c>
+      <c r="D141" s="1">
+        <v>44137</v>
+      </c>
+      <c r="E141" t="s">
+        <v>602</v>
+      </c>
+      <c r="F141" t="s">
+        <v>16</v>
+      </c>
+      <c r="G141" t="s">
+        <v>603</v>
+      </c>
+      <c r="H141">
+        <v>3</v>
+      </c>
+      <c r="I141" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6280,13 +6321,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -6297,7 +6338,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>452</v>
       </c>
@@ -6308,7 +6349,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>452</v>
       </c>
@@ -6319,7 +6360,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>452</v>
       </c>
@@ -6330,7 +6371,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -6341,7 +6382,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>452</v>
       </c>
@@ -6365,13 +6406,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6379,7 +6420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -6387,7 +6428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1776</v>
       </c>
@@ -6395,7 +6436,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -6403,7 +6444,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -6411,7 +6452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -6419,7 +6460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -6427,7 +6468,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -6435,7 +6476,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -6443,7 +6484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -6451,7 +6492,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -6459,7 +6500,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -6467,7 +6508,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -6475,7 +6516,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -6483,7 +6524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -6491,7 +6532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -6499,7 +6540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -6507,7 +6548,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -6515,7 +6556,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -6523,7 +6564,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -6531,7 +6572,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -6539,7 +6580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
added the killer across the table
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD38C31A-0EBF-4E2F-93FF-9CA7E64B45D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431EF665-E1B2-4E78-B139-B9C1E7C8881A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="612">
   <si>
     <t>Title</t>
   </si>
@@ -1859,6 +1859,18 @@
   </si>
   <si>
     <t>8 Hours 20 Mins</t>
+  </si>
+  <si>
+    <t>The Killer Across the Table</t>
+  </si>
+  <si>
+    <t>John E. Douglas</t>
+  </si>
+  <si>
+    <t>serial killers;psychology;history</t>
+  </si>
+  <si>
+    <t>11 Hours 7 Mins</t>
   </si>
 </sst>
 </file>
@@ -2214,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:I143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6346,6 +6358,35 @@
         <v>3</v>
       </c>
       <c r="I142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>608</v>
+      </c>
+      <c r="B143" t="s">
+        <v>609</v>
+      </c>
+      <c r="C143" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D143" s="1">
+        <v>44140</v>
+      </c>
+      <c r="E143" t="s">
+        <v>610</v>
+      </c>
+      <c r="F143" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" t="s">
+        <v>611</v>
+      </c>
+      <c r="H143">
+        <v>3</v>
+      </c>
+      <c r="I143" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added skunk works and tiger woods
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E817B02-EFE2-4011-B386-129C0B3C4FF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7EF82-54C9-4F1F-9F90-9D067424AAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="623">
   <si>
     <t>Title</t>
   </si>
@@ -1883,6 +1883,27 @@
   </si>
   <si>
     <t>9 Hours 54 Mins</t>
+  </si>
+  <si>
+    <t>Skunk Works</t>
+  </si>
+  <si>
+    <t>Ben Rich</t>
+  </si>
+  <si>
+    <t>memoir;aerospace;stealth;technology;business</t>
+  </si>
+  <si>
+    <t>Tiger Woods</t>
+  </si>
+  <si>
+    <t>Jeff Benedict</t>
+  </si>
+  <si>
+    <t>15 Hours 23 Mins</t>
+  </si>
+  <si>
+    <t>biography;tiger woods;greatness;scandal;golf;sports;champion</t>
   </si>
 </sst>
 </file>
@@ -2238,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6428,6 +6449,64 @@
         <v>3</v>
       </c>
       <c r="I144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>616</v>
+      </c>
+      <c r="B145" t="s">
+        <v>617</v>
+      </c>
+      <c r="C145" s="1">
+        <v>44142</v>
+      </c>
+      <c r="D145" s="1">
+        <v>44146</v>
+      </c>
+      <c r="E145" t="s">
+        <v>618</v>
+      </c>
+      <c r="F145" t="s">
+        <v>16</v>
+      </c>
+      <c r="G145" t="s">
+        <v>297</v>
+      </c>
+      <c r="H145">
+        <v>3</v>
+      </c>
+      <c r="I145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>619</v>
+      </c>
+      <c r="B146" t="s">
+        <v>620</v>
+      </c>
+      <c r="C146" s="1">
+        <v>44146</v>
+      </c>
+      <c r="D146" s="1">
+        <v>44152</v>
+      </c>
+      <c r="E146" t="s">
+        <v>622</v>
+      </c>
+      <c r="F146" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" t="s">
+        <v>621</v>
+      </c>
+      <c r="H146">
+        <v>4</v>
+      </c>
+      <c r="I146" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added seinfeldia and catherine the great
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7EF82-54C9-4F1F-9F90-9D067424AAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E507CF-F705-491E-8BF0-5239B27C1B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="631">
   <si>
     <t>Title</t>
   </si>
@@ -1904,6 +1904,30 @@
   </si>
   <si>
     <t>biography;tiger woods;greatness;scandal;golf;sports;champion</t>
+  </si>
+  <si>
+    <t>Seinfeldia</t>
+  </si>
+  <si>
+    <t>Jennifer Keishin Armstrong</t>
+  </si>
+  <si>
+    <t>seinfeld;tv;history;comedy;writing</t>
+  </si>
+  <si>
+    <t>9 Hours 59 Mins</t>
+  </si>
+  <si>
+    <t>Catherine The Great</t>
+  </si>
+  <si>
+    <t>Robert Massie</t>
+  </si>
+  <si>
+    <t>catherine the great;russia;18th century;autocracy;history;biography</t>
+  </si>
+  <si>
+    <t>23 Hours 52 Mins</t>
   </si>
 </sst>
 </file>
@@ -2259,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6508,6 +6532,64 @@
       </c>
       <c r="I146" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>623</v>
+      </c>
+      <c r="B147" t="s">
+        <v>624</v>
+      </c>
+      <c r="C147" s="1">
+        <v>44158</v>
+      </c>
+      <c r="D147" s="1">
+        <v>44162</v>
+      </c>
+      <c r="E147" t="s">
+        <v>625</v>
+      </c>
+      <c r="F147" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" t="s">
+        <v>626</v>
+      </c>
+      <c r="H147">
+        <v>3</v>
+      </c>
+      <c r="I147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>627</v>
+      </c>
+      <c r="B148" t="s">
+        <v>628</v>
+      </c>
+      <c r="C148" s="1">
+        <v>44162</v>
+      </c>
+      <c r="D148" s="1">
+        <v>44169</v>
+      </c>
+      <c r="E148" t="s">
+        <v>629</v>
+      </c>
+      <c r="F148" t="s">
+        <v>16</v>
+      </c>
+      <c r="G148" t="s">
+        <v>630</v>
+      </c>
+      <c r="H148">
+        <v>3</v>
+      </c>
+      <c r="I148" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added jack straight from the gut
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FE021B-1194-42DC-B619-75F74187BD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1CFA2C-F566-41E1-A521-6F2189F62805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="640">
   <si>
     <t>Title</t>
   </si>
@@ -1940,6 +1940,21 @@
   </si>
   <si>
     <t>11 Hours 54 Mins</t>
+  </si>
+  <si>
+    <t>Jack: Straight from the Gut</t>
+  </si>
+  <si>
+    <t>Jack Welch</t>
+  </si>
+  <si>
+    <t>10/30/202</t>
+  </si>
+  <si>
+    <t>jack welch;biography;memoir;ge;business</t>
+  </si>
+  <si>
+    <t>437 Pages</t>
   </si>
 </sst>
 </file>
@@ -2295,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6630,6 +6645,35 @@
         <v>4</v>
       </c>
       <c r="I149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>635</v>
+      </c>
+      <c r="B150" t="s">
+        <v>636</v>
+      </c>
+      <c r="C150" t="s">
+        <v>637</v>
+      </c>
+      <c r="D150" s="1">
+        <v>44174</v>
+      </c>
+      <c r="E150" t="s">
+        <v>638</v>
+      </c>
+      <c r="F150" t="s">
+        <v>17</v>
+      </c>
+      <c r="G150" t="s">
+        <v>639</v>
+      </c>
+      <c r="H150">
+        <v>3</v>
+      </c>
+      <c r="I150" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Thicker than Water
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1CFA2C-F566-41E1-A521-6F2189F62805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D955EB56-A0F3-491F-B077-7327BFD1F1C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="643">
   <si>
     <t>Title</t>
   </si>
@@ -1948,13 +1948,22 @@
     <t>Jack Welch</t>
   </si>
   <si>
-    <t>10/30/202</t>
-  </si>
-  <si>
     <t>jack welch;biography;memoir;ge;business</t>
   </si>
   <si>
     <t>437 Pages</t>
+  </si>
+  <si>
+    <t>Thicker than Water</t>
+  </si>
+  <si>
+    <t>Tyler Schultz</t>
+  </si>
+  <si>
+    <t>theranos;elizabeth holmes;fraud;business</t>
+  </si>
+  <si>
+    <t>3 Hours 37 Mins</t>
   </si>
 </sst>
 </file>
@@ -2310,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
-  <dimension ref="A1:I150"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6655,25 +6664,54 @@
       <c r="B150" t="s">
         <v>636</v>
       </c>
-      <c r="C150" t="s">
-        <v>637</v>
+      <c r="C150" s="1">
+        <v>44134</v>
       </c>
       <c r="D150" s="1">
         <v>44174</v>
       </c>
       <c r="E150" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F150" t="s">
         <v>17</v>
       </c>
       <c r="G150" t="s">
+        <v>638</v>
+      </c>
+      <c r="H150">
+        <v>3</v>
+      </c>
+      <c r="I150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>639</v>
       </c>
-      <c r="H150">
-        <v>3</v>
-      </c>
-      <c r="I150" t="b">
+      <c r="B151" t="s">
+        <v>640</v>
+      </c>
+      <c r="C151" s="1">
+        <v>44196</v>
+      </c>
+      <c r="D151" s="1">
+        <v>44196</v>
+      </c>
+      <c r="E151" t="s">
+        <v>641</v>
+      </c>
+      <c r="F151" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" t="s">
+        <v>642</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+      <c r="I151" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created book list for 2021
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D955EB56-A0F3-491F-B077-7327BFD1F1C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C623ECAF-0F4A-42B9-AD39-F703A4B8C816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="1" r:id="rId1"/>
@@ -1970,8 +1970,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1999,12 +2007,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2321,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44DAC96-81A0-454C-8C35-E5A37D2893EB}">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6809,8 +6821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDDD9D0-399A-4972-B572-FF4C9ED18E5D}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6988,14 +7000,15 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added harry potter 3 and hard thing about hard things
</commit_message>
<xml_diff>
--- a/book_list.xlsx
+++ b/book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C623ECAF-0F4A-42B9-AD39-F703A4B8C816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA51C9-C3AD-45FF-A5C1-DA8CCAF9BC94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3D47C23-FD95-4BA6-9A71-BF3A0BF9343C}"/>
   </bookViews>
@@ -6821,8 +6821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDDD9D0-399A-4972-B572-FF4C9ED18E5D}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6864,10 +6864,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6880,10 +6880,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>